<commit_message>
added LeafGrowthRate and LeafSenescenceRate
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -33,13 +33,14 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="614">
   <si>
     <t>name.rsunflo.fr</t>
   </si>
@@ -1133,7 +1134,13 @@
     <t>LAI_d</t>
   </si>
   <si>
+    <t>PotentialLeafDuration</t>
+  </si>
+  <si>
     <t>Valeur du maximum de la fonction de la durée de vie des feuilles en fonction du rang sur la tige</t>
+  </si>
+  <si>
+    <t>Thermal time between expansion and senescence</t>
   </si>
   <si>
     <t>LAI_e</t>
@@ -2152,8 +2159,8 @@
   </sheetPr>
   <dimension ref="1:102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -4666,11 +4673,20 @@
       <c r="D67" s="0" t="s">
         <v>334</v>
       </c>
+      <c r="E67" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="F67" s="0" t="s">
         <v>363</v>
       </c>
+      <c r="I67" s="0" t="s">
+        <v>364</v>
+      </c>
       <c r="J67" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>366</v>
       </c>
       <c r="L67" s="3" t="s">
         <v>47</v>
@@ -4696,10 +4712,10 @@
         <v>334</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>69</v>
@@ -4725,10 +4741,10 @@
         <v>334</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>69</v>
@@ -4754,10 +4770,10 @@
         <v>334</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="L70" s="3" t="s">
         <v>86</v>
@@ -4783,13 +4799,13 @@
         <v>334</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M71" s="0" t="s">
         <v>107</v>
@@ -4812,13 +4828,13 @@
         <v>334</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="J72" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="L72" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>373</v>
       </c>
       <c r="M72" s="0" t="s">
         <v>107</v>
@@ -4841,13 +4857,13 @@
         <v>334</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M73" s="0" t="s">
         <v>107</v>
@@ -4870,13 +4886,13 @@
         <v>334</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M74" s="0" t="s">
         <v>107</v>
@@ -4899,10 +4915,10 @@
         <v>334</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="L75" s="3" t="s">
         <v>9</v>
@@ -4928,10 +4944,10 @@
         <v>334</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="K76" s="3"/>
       <c r="L76" s="3" t="s">
@@ -4958,10 +4974,10 @@
         <v>334</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="K77" s="3"/>
       <c r="L77" s="3" t="s">
@@ -4988,10 +5004,10 @@
         <v>334</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="L78" s="3" t="s">
         <v>86</v>
@@ -5017,10 +5033,10 @@
         <v>334</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="L79" s="3" t="s">
         <v>47</v>
@@ -5046,10 +5062,10 @@
         <v>334</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="L80" s="3" t="s">
         <v>86</v>
@@ -5072,19 +5088,19 @@
         <v>333</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>133</v>
       </c>
       <c r="M81" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N81" s="4" t="n">
         <v>4.53</v>
@@ -5101,19 +5117,19 @@
         <v>333</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>86</v>
       </c>
       <c r="M82" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N82" s="4" t="n">
         <v>0.42</v>
@@ -5130,19 +5146,19 @@
         <v>333</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="L83" s="3" t="s">
         <v>133</v>
       </c>
       <c r="M83" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N83" s="4" t="n">
         <v>6.49</v>
@@ -5159,19 +5175,19 @@
         <v>333</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="L84" s="3" t="s">
         <v>86</v>
       </c>
       <c r="M84" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N84" s="4" t="n">
         <v>0.44</v>
@@ -5188,19 +5204,19 @@
         <v>333</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="J85" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="M85" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N85" s="4" t="n">
         <v>75</v>
@@ -5217,19 +5233,19 @@
         <v>333</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="J86" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="L86" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="L86" s="3" t="s">
-        <v>404</v>
-      </c>
       <c r="M86" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N86" s="4" t="n">
         <v>75</v>
@@ -5246,19 +5262,19 @@
         <v>333</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="J87" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="L87" s="3" t="s">
         <v>86</v>
       </c>
       <c r="M87" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="N87" s="4" t="n">
         <v>0.6</v>
@@ -5275,19 +5291,19 @@
         <v>333</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="L88" s="3" t="s">
         <v>86</v>
       </c>
       <c r="M88" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="N88" s="4" t="n">
         <v>0.3</v>
@@ -5304,16 +5320,16 @@
         <v>333</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="J89" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="M89" s="0" t="s">
         <v>48</v>
@@ -5333,13 +5349,13 @@
         <v>333</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="J90" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="L90" s="3" t="s">
         <v>86</v>
@@ -5359,13 +5375,13 @@
         <v>333</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J91" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="L91" s="3" t="s">
         <v>86</v>
@@ -5388,25 +5404,25 @@
         <v>333</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E92" s="0" t="s">
         <v>41</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I92" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="K92" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="M92" s="0" t="s">
         <v>342</v>
@@ -5423,13 +5439,13 @@
         <v>100</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="L93" s="3"/>
       <c r="P93" s="0" t="n">
@@ -5441,13 +5457,13 @@
         <v>101</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="L94" s="3"/>
       <c r="P94" s="0" t="n">
@@ -5459,13 +5475,13 @@
         <v>102</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="L95" s="3"/>
       <c r="P95" s="0" t="n">
@@ -5477,13 +5493,13 @@
         <v>103</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="L96" s="3"/>
       <c r="P96" s="0" t="n">
@@ -5495,13 +5511,13 @@
         <v>104</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="L97" s="3"/>
       <c r="P97" s="0" t="n">
@@ -5513,13 +5529,13 @@
         <v>105</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="L98" s="3"/>
       <c r="P98" s="0" t="n">
@@ -5531,13 +5547,13 @@
         <v>106</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="L99" s="3"/>
       <c r="P99" s="0" t="n">
@@ -5549,13 +5565,13 @@
         <v>107</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="L100" s="3"/>
       <c r="P100" s="0" t="n">
@@ -5567,13 +5583,13 @@
         <v>108</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="L101" s="3"/>
       <c r="P101" s="0" t="n">
@@ -5585,13 +5601,13 @@
         <v>109</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="P102" s="0" t="n">
         <v>0</v>
@@ -5659,7 +5675,7 @@
         <v>41</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5667,7 +5683,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5675,7 +5691,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5683,7 +5699,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5691,7 +5707,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5699,7 +5715,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5707,7 +5723,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5720,42 +5736,42 @@
     </row>
     <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -5797,10 +5813,10 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>32</v>
@@ -5815,7 +5831,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5823,19 +5839,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>9</v>
@@ -5849,19 +5865,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>9</v>
@@ -5875,19 +5891,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>9</v>
@@ -5901,13 +5917,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -5916,7 +5932,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>1</v>
@@ -5927,13 +5943,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
@@ -5953,13 +5969,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -5979,22 +5995,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>1</v>
@@ -6005,19 +6021,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>86</v>
@@ -6031,19 +6047,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>86</v>
@@ -6057,19 +6073,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>86</v>
@@ -6083,19 +6099,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>86</v>
@@ -6109,19 +6125,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>86</v>
@@ -6135,19 +6151,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>86</v>
@@ -6161,22 +6177,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>1</v>
@@ -6187,19 +6203,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>86</v>
@@ -6213,19 +6229,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>86</v>
@@ -6239,19 +6255,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>86</v>
@@ -6265,19 +6281,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>86</v>
@@ -6291,19 +6307,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>86</v>
@@ -6317,22 +6333,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>1</v>
@@ -6343,22 +6359,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>1</v>
@@ -6369,19 +6385,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>109</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>113</v>
@@ -6431,22 +6447,22 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -6458,7 +6474,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6466,34 +6482,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6501,34 +6517,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6536,34 +6552,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6571,34 +6587,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6606,34 +6622,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6641,34 +6657,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6676,34 +6692,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6711,34 +6727,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6746,34 +6762,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6781,34 +6797,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6816,34 +6832,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6851,34 +6867,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6886,34 +6902,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6921,34 +6937,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>86</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6956,34 +6972,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6991,34 +7007,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7026,34 +7042,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7061,34 +7077,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7096,34 +7112,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7131,34 +7147,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>109</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added output variable section, started WaterStress section.
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="286" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="233" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,13 +41,14 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="650">
   <si>
     <t>name.rsunflo.fr</t>
   </si>
@@ -1468,9 +1469,15 @@
     <t>TM</t>
   </si>
   <si>
+    <t>TemperatureAirMean</t>
+  </si>
+  <si>
     <t>Température moyenne</t>
   </si>
   <si>
+    <t>Mean air temperature</t>
+  </si>
+  <si>
     <t>RG</t>
   </si>
   <si>
@@ -1498,424 +1505,493 @@
     <t>Temps thermique cumulé depuis la levée</t>
   </si>
   <si>
+    <t>Temperature sum from emergence</t>
+  </si>
+  <si>
+    <t>PhasePhenoPlante</t>
+  </si>
+  <si>
+    <t>PhenoStage</t>
+  </si>
+  <si>
+    <t>Index de phénologie</t>
+  </si>
+  <si>
+    <t>Phenological stages index </t>
+  </si>
+  <si>
+    <t>contrainte_eau</t>
+  </si>
+  <si>
+    <t>FTSW</t>
+  </si>
+  <si>
+    <t>WaterStress</t>
+  </si>
+  <si>
+    <t>Facteur de contrainte hydrique</t>
+  </si>
+  <si>
+    <t>Water stress index</t>
+  </si>
+  <si>
+    <t>FHTR</t>
+  </si>
+  <si>
+    <t>WaterStressConductance</t>
+  </si>
+  <si>
+    <t>Facteur de réponse de la transpiration à la contrainte hydrique</t>
+  </si>
+  <si>
+    <t>Transpiration response to water stress</t>
+  </si>
+  <si>
+    <t>FHRUE</t>
+  </si>
+  <si>
+    <t>Facteur de réponse de la photosynthèse à la contrainte hydrique</t>
+  </si>
+  <si>
+    <t>Photosynthesis response to water stress</t>
+  </si>
+  <si>
+    <t>ETRETM</t>
+  </si>
+  <si>
+    <t>WaterSupplyDemandRatio</t>
+  </si>
+  <si>
+    <t>Ratio ETR/ETM</t>
+  </si>
+  <si>
+    <t>Water supply:demand ratio</t>
+  </si>
+  <si>
+    <t>contrainte_temperature</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>FTRUE</t>
+  </si>
+  <si>
+    <t>ThermalStressRUE</t>
+  </si>
+  <si>
+    <t>Facteur de réponse de la photosynthèse à la contrainte thermique</t>
+  </si>
+  <si>
+    <t>Photosynthesis response to thermal stress</t>
+  </si>
+  <si>
+    <t>contrainte_azote</t>
+  </si>
+  <si>
+    <t>Nabs</t>
+  </si>
+  <si>
+    <t>NAB</t>
+  </si>
+  <si>
+    <t>NitrogenAbsorbed</t>
+  </si>
+  <si>
+    <t>Azote absorbé</t>
+  </si>
+  <si>
+    <t>Absorbed nitrogen</t>
+  </si>
+  <si>
+    <t>kg.ha-1.d-1</t>
+  </si>
+  <si>
+    <t>INN</t>
+  </si>
+  <si>
+    <t>NNI</t>
+  </si>
+  <si>
+    <t>NitrogenNutritionIndex</t>
+  </si>
+  <si>
+    <t>Indice de nutrition azoté</t>
+  </si>
+  <si>
+    <t>Nitrogen nutrition index</t>
+  </si>
+  <si>
+    <t>FNIRUE</t>
+  </si>
+  <si>
+    <t>FNRUE</t>
+  </si>
+  <si>
+    <t>NitrogenStressRUE</t>
+  </si>
+  <si>
+    <t>Facteur de réponse de la photosynthèse à la contrainte azote</t>
+  </si>
+  <si>
+    <t>Photosynthesis response to nitrogen stress</t>
+  </si>
+  <si>
+    <t>croissance_plante</t>
+  </si>
+  <si>
+    <t>Indice foliaire</t>
+  </si>
+  <si>
+    <t>Leaf area index</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>Efficience d'interception de la lumière</t>
+  </si>
+  <si>
+    <t>Radiation interception efficiency</t>
+  </si>
+  <si>
+    <t>Eb</t>
+  </si>
+  <si>
+    <t>Efficience d'utilisation de la lumière</t>
+  </si>
+  <si>
+    <t>Radiation use efficiency</t>
+  </si>
+  <si>
+    <t>TDM</t>
+  </si>
+  <si>
+    <t>Biomasse aérienne</t>
+  </si>
+  <si>
+    <t>Crop aerial dry biomass</t>
+  </si>
+  <si>
+    <t>g.m-2</t>
+  </si>
+  <si>
+    <t>elaboration_rendement</t>
+  </si>
+  <si>
+    <t>photo_RDT_aFinMATURATION</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>CropYield</t>
+  </si>
+  <si>
+    <t>Rendement en grain</t>
+  </si>
+  <si>
+    <t>Grain yield</t>
+  </si>
+  <si>
+    <t>q.ha-1</t>
+  </si>
+  <si>
+    <t>elaboration_qualite</t>
+  </si>
+  <si>
+    <t>photo_TH_aFinMATURATION</t>
+  </si>
+  <si>
+    <t>OilContent</t>
+  </si>
+  <si>
+    <t>Teneur en huile</t>
+  </si>
+  <si>
+    <t>Grain oil content</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>climate</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>photosynthesis</t>
+  </si>
+  <si>
+    <t>SGR</t>
+  </si>
+  <si>
+    <t>cycle</t>
+  </si>
+  <si>
+    <t>Rayonnement incident (PAR)</t>
+  </si>
+  <si>
+    <t>Photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>sum(GR*0.48)</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>SRR</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>sum(RR)</t>
+  </si>
+  <si>
+    <t>SETP</t>
+  </si>
+  <si>
+    <t>Evapotranspiration</t>
+  </si>
+  <si>
+    <t>Potential evapotranspiration</t>
+  </si>
+  <si>
+    <t>sum(ETP)</t>
+  </si>
+  <si>
+    <t>SCWD</t>
+  </si>
+  <si>
+    <t>Déficit hydrique climatique</t>
+  </si>
+  <si>
+    <t>Climatic water deficit</t>
+  </si>
+  <si>
+    <t>sum(P-ETP)</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>SFTSW</t>
+  </si>
+  <si>
+    <t>Déficit hydrique édaphique (continu)</t>
+  </si>
+  <si>
+    <t>Edaphic water deficit (continuous)</t>
+  </si>
+  <si>
+    <t>sum(1-FTSW)</t>
+  </si>
+  <si>
+    <t>NETR</t>
+  </si>
+  <si>
+    <t>Déficit hydrique édaphique (discret)</t>
+  </si>
+  <si>
+    <t>Edaphic water deficit (discrete)</t>
+  </si>
+  <si>
+    <t>sum(ETR/ETM &lt; 0.6)</t>
+  </si>
+  <si>
+    <t>transpiration</t>
+  </si>
+  <si>
+    <t>SFHTR</t>
+  </si>
+  <si>
+    <t>Effet de la contrainte hydrique sur la transpiration</t>
+  </si>
+  <si>
+    <t>Water stress impact on crop transpiration</t>
+  </si>
+  <si>
+    <t>sum(1-FHTR)</t>
+  </si>
+  <si>
+    <t>SFHRUE</t>
+  </si>
+  <si>
+    <t>Effet de la contrainte hydrique sur la photosynthèse</t>
+  </si>
+  <si>
+    <t>Water stress impact on crop photosynthesis</t>
+  </si>
+  <si>
+    <t>sum(1-FHRUE)</t>
+  </si>
+  <si>
+    <t>nitrogen</t>
+  </si>
+  <si>
+    <t>SNNI</t>
+  </si>
+  <si>
+    <t>Déficit azoté</t>
+  </si>
+  <si>
+    <t>Nitrogen deficit</t>
+  </si>
+  <si>
+    <t>sum(1-NNI)</t>
+  </si>
+  <si>
+    <t>SNAB</t>
+  </si>
+  <si>
+    <t>kg/ha</t>
+  </si>
+  <si>
+    <t>diff(range(NAB))</t>
+  </si>
+  <si>
+    <t>SFNRUE</t>
+  </si>
+  <si>
+    <t>Effet de la contrainte azote sur la photosynthèse</t>
+  </si>
+  <si>
+    <t>Nitrogen stress impact on photosynthesis</t>
+  </si>
+  <si>
+    <t>sum(1-FNRUE)</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>SFTRUE</t>
+  </si>
+  <si>
+    <t>Effet de la contrainte thermique sur la photosynthèse</t>
+  </si>
+  <si>
+    <t>Thermal stress impact on photosynthesis</t>
+  </si>
+  <si>
+    <t>sum(1-FTRUE)</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>interception</t>
+  </si>
+  <si>
+    <t>Indice foliaire maximum</t>
+  </si>
+  <si>
+    <t>max(LAI)</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>Durée de surface foliaire</t>
+  </si>
+  <si>
+    <t>Leaf area duration</t>
+  </si>
+  <si>
+    <t>sum(LAI)</t>
+  </si>
+  <si>
+    <t>SIR</t>
+  </si>
+  <si>
+    <t>Rayonnement intercepté (PAR)</t>
+  </si>
+  <si>
+    <t>Intercepted radiation</t>
+  </si>
+  <si>
+    <t>sum(RIE*GR*0.48)</t>
+  </si>
+  <si>
+    <t>MRUE</t>
+  </si>
+  <si>
+    <t>Photosynthèse</t>
+  </si>
+  <si>
+    <t>Photosynthesis</t>
+  </si>
+  <si>
+    <t>g/MJ/m2</t>
+  </si>
+  <si>
+    <t>mean(RUE)</t>
+  </si>
+  <si>
+    <t>STDM</t>
+  </si>
+  <si>
+    <t>Biomasse</t>
+  </si>
+  <si>
+    <t>Aerial Biomass</t>
+  </si>
+  <si>
+    <t>max(TDM)</t>
+  </si>
+  <si>
+    <t>ressource</t>
+  </si>
+  <si>
+    <t>phenology</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Temps thermique (base 4.8°C)</t>
+  </si>
+  <si>
+    <t>Thermal time</t>
+  </si>
+  <si>
     <t>°C.j</t>
   </si>
   <si>
-    <t>PhasePhenoPlante</t>
-  </si>
-  <si>
-    <t>PhenoStage</t>
-  </si>
-  <si>
-    <t>Index de phénologie</t>
-  </si>
-  <si>
-    <t>contrainte_eau</t>
-  </si>
-  <si>
-    <t>FTSW</t>
-  </si>
-  <si>
-    <t>Facteur de contrainte hydrique</t>
-  </si>
-  <si>
-    <t>FHTR</t>
-  </si>
-  <si>
-    <t>Facteur de réponse de la transpiration à la contrainte hydrique</t>
-  </si>
-  <si>
-    <t>FHRUE</t>
-  </si>
-  <si>
-    <t>Facteur de réponse de la photosynthèse à la contrainte hydrique</t>
-  </si>
-  <si>
-    <t>ETRETM</t>
-  </si>
-  <si>
-    <t>Ratio ETR/ETM</t>
-  </si>
-  <si>
-    <t>contrainte_temperature</t>
-  </si>
-  <si>
-    <t>FT</t>
-  </si>
-  <si>
-    <t>FTRUE</t>
-  </si>
-  <si>
-    <t>Facteur de réponse de la photosynthèse à la contrainte thermique</t>
-  </si>
-  <si>
-    <t>contrainte_azote</t>
-  </si>
-  <si>
-    <t>Nabs</t>
-  </si>
-  <si>
-    <t>NAB</t>
-  </si>
-  <si>
-    <t>Azote absorbé</t>
-  </si>
-  <si>
-    <t>kg/ha/j</t>
-  </si>
-  <si>
-    <t>INN</t>
-  </si>
-  <si>
-    <t>NNI</t>
-  </si>
-  <si>
-    <t>Indice de nutrition azoté</t>
-  </si>
-  <si>
-    <t>FNIRUE</t>
-  </si>
-  <si>
-    <t>FNRUE</t>
-  </si>
-  <si>
-    <t>Facteur de réponse de la photosynthèse à la contrainte azote</t>
-  </si>
-  <si>
-    <t>croissance_plante</t>
-  </si>
-  <si>
-    <t>Indice foliaire</t>
-  </si>
-  <si>
-    <t>Ei</t>
-  </si>
-  <si>
-    <t>Efficience d'interception de la lumière</t>
-  </si>
-  <si>
-    <t>Eb</t>
-  </si>
-  <si>
-    <t>Efficience d'utilisation de la lumière</t>
-  </si>
-  <si>
-    <t>TDM</t>
-  </si>
-  <si>
-    <t>Biomasse aérienne</t>
-  </si>
-  <si>
-    <t>elaboration_rendement</t>
-  </si>
-  <si>
-    <t>photo_RDT_aFinMATURATION</t>
-  </si>
-  <si>
-    <t>GY</t>
-  </si>
-  <si>
-    <t>Rendement en grain</t>
+    <t>max(TTA2)</t>
+  </si>
+  <si>
+    <t>performance</t>
   </si>
   <si>
     <t>q/ha</t>
   </si>
   <si>
-    <t>elaboration_qualite</t>
-  </si>
-  <si>
-    <t>photo_TH_aFinMATURATION</t>
-  </si>
-  <si>
-    <t>Teneur en huile</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>factor</t>
-  </si>
-  <si>
-    <t>process</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>formula</t>
-  </si>
-  <si>
-    <t>resource</t>
-  </si>
-  <si>
-    <t>climate</t>
-  </si>
-  <si>
-    <t>light</t>
-  </si>
-  <si>
-    <t>photosynthesis</t>
-  </si>
-  <si>
-    <t>SGR</t>
-  </si>
-  <si>
-    <t>cycle</t>
-  </si>
-  <si>
-    <t>Rayonnement incident (PAR)</t>
-  </si>
-  <si>
-    <t>Photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>sum(GR*0.48)</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>SRR</t>
-  </si>
-  <si>
-    <t>Rain</t>
-  </si>
-  <si>
-    <t>sum(RR)</t>
-  </si>
-  <si>
-    <t>SETP</t>
-  </si>
-  <si>
-    <t>Evapotranspiration</t>
-  </si>
-  <si>
-    <t>Potential evapotranspiration</t>
-  </si>
-  <si>
-    <t>sum(ETP)</t>
-  </si>
-  <si>
-    <t>SCWD</t>
-  </si>
-  <si>
-    <t>Déficit hydrique climatique</t>
-  </si>
-  <si>
-    <t>Climatic water deficit</t>
-  </si>
-  <si>
-    <t>sum(P-ETP)</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>crop</t>
-  </si>
-  <si>
-    <t>SFTSW</t>
-  </si>
-  <si>
-    <t>Déficit hydrique édaphique (continu)</t>
-  </si>
-  <si>
-    <t>Edaphic water deficit (continuous)</t>
-  </si>
-  <si>
-    <t>sum(1-FTSW)</t>
-  </si>
-  <si>
-    <t>NETR</t>
-  </si>
-  <si>
-    <t>Déficit hydrique édaphique (discret)</t>
-  </si>
-  <si>
-    <t>Edaphic water deficit (discrete)</t>
-  </si>
-  <si>
-    <t>sum(ETR/ETM &lt; 0.6)</t>
-  </si>
-  <si>
-    <t>transpiration</t>
-  </si>
-  <si>
-    <t>SFHTR</t>
-  </si>
-  <si>
-    <t>Effet de la contrainte hydrique sur la transpiration</t>
-  </si>
-  <si>
-    <t>Water stress impact on crop transpiration</t>
-  </si>
-  <si>
-    <t>sum(1-FHTR)</t>
-  </si>
-  <si>
-    <t>SFHRUE</t>
-  </si>
-  <si>
-    <t>Effet de la contrainte hydrique sur la photosynthèse</t>
-  </si>
-  <si>
-    <t>Water stress impact on crop photosynthesis</t>
-  </si>
-  <si>
-    <t>sum(1-FHRUE)</t>
-  </si>
-  <si>
-    <t>nitrogen</t>
-  </si>
-  <si>
-    <t>SNNI</t>
-  </si>
-  <si>
-    <t>Déficit azoté</t>
-  </si>
-  <si>
-    <t>Nitrogen deficit</t>
-  </si>
-  <si>
-    <t>sum(1-NNI)</t>
-  </si>
-  <si>
-    <t>SNAB</t>
-  </si>
-  <si>
-    <t>Absorbed nitrogen</t>
-  </si>
-  <si>
-    <t>kg/ha</t>
-  </si>
-  <si>
-    <t>diff(range(NAB))</t>
-  </si>
-  <si>
-    <t>SFNRUE</t>
-  </si>
-  <si>
-    <t>Effet de la contrainte azote sur la photosynthèse</t>
-  </si>
-  <si>
-    <t>Nitrogen stress impact on photosynthesis</t>
-  </si>
-  <si>
-    <t>sum(1-FNRUE)</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>SFTRUE</t>
-  </si>
-  <si>
-    <t>Effet de la contrainte thermique sur la photosynthèse</t>
-  </si>
-  <si>
-    <t>Thermal stress impact on photosynthesis</t>
-  </si>
-  <si>
-    <t>sum(1-FTRUE)</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>interception</t>
-  </si>
-  <si>
-    <t>Indice foliaire maximum</t>
-  </si>
-  <si>
-    <t>Leaf area index</t>
-  </si>
-  <si>
-    <t>max(LAI)</t>
-  </si>
-  <si>
-    <t>DSF</t>
-  </si>
-  <si>
-    <t>Durée de surface foliaire</t>
-  </si>
-  <si>
-    <t>Leaf area duration</t>
-  </si>
-  <si>
-    <t>sum(LAI)</t>
-  </si>
-  <si>
-    <t>SIR</t>
-  </si>
-  <si>
-    <t>Rayonnement intercepté (PAR)</t>
-  </si>
-  <si>
-    <t>Intercepted radiation</t>
-  </si>
-  <si>
-    <t>sum(RIE*GR*0.48)</t>
-  </si>
-  <si>
-    <t>MRUE</t>
-  </si>
-  <si>
-    <t>Photosynthèse</t>
-  </si>
-  <si>
-    <t>Photosynthesis</t>
-  </si>
-  <si>
-    <t>g/MJ/m2</t>
-  </si>
-  <si>
-    <t>mean(RUE)</t>
-  </si>
-  <si>
-    <t>STDM</t>
-  </si>
-  <si>
-    <t>Biomasse</t>
-  </si>
-  <si>
-    <t>Aerial Biomass</t>
-  </si>
-  <si>
-    <t>max(TDM)</t>
-  </si>
-  <si>
-    <t>ressource</t>
-  </si>
-  <si>
-    <t>phenology</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>Temps thermique (base 4.8°C)</t>
-  </si>
-  <si>
-    <t>Thermal time</t>
-  </si>
-  <si>
-    <t>max(TTA2)</t>
-  </si>
-  <si>
-    <t>performance</t>
-  </si>
-  <si>
-    <t>Grain yield</t>
-  </si>
-  <si>
     <t>max(GY)</t>
-  </si>
-  <si>
-    <t>Grain oil content</t>
   </si>
   <si>
     <t>% (DM)</t>
@@ -2068,7 +2144,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -2201,8 +2277,8 @@
   </sheetPr>
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -7687,25 +7763,27 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.2"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6377551020408"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1428571428571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.7704081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.3826530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.6377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.3826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -7722,16 +7800,22 @@
         <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -7748,16 +7832,22 @@
         <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -7774,16 +7864,22 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -7803,13 +7899,19 @@
         <v>473</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -7820,22 +7922,28 @@
         <v>466</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -7846,22 +7954,28 @@
         <v>466</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -7872,290 +7986,356 @@
         <v>466</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="H7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>484</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>487</v>
       </c>
       <c r="G9" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>492</v>
       </c>
       <c r="G10" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>496</v>
       </c>
       <c r="G11" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>493</v>
+        <v>499</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>496</v>
       </c>
       <c r="G12" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>495</v>
+        <v>502</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>503</v>
       </c>
       <c r="G13" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>499</v>
+        <v>508</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>509</v>
       </c>
       <c r="G14" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>503</v>
+        <v>514</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>515</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>504</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>516</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>507</v>
+        <v>520</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>521</v>
       </c>
       <c r="G16" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>508</v>
+        <v>524</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>510</v>
+        <v>525</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>526</v>
       </c>
       <c r="G17" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>458</v>
@@ -8163,143 +8343,179 @@
       <c r="E18" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>512</v>
+      <c r="F18" s="3" t="s">
+        <v>458</v>
       </c>
       <c r="G18" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="I18" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>513</v>
+        <v>532</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>514</v>
+      <c r="F19" s="3" t="s">
+        <v>459</v>
       </c>
       <c r="G19" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>516</v>
+      <c r="F20" s="3" t="s">
+        <v>461</v>
       </c>
       <c r="G20" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>517</v>
+        <v>538</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>518</v>
+        <v>538</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>460</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>539</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>519</v>
+        <v>542</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>522</v>
+        <v>544</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>545</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>546</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>524</v>
+        <v>549</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>525</v>
+        <v>550</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>526</v>
+      <c r="F23" s="3" t="s">
+        <v>551</v>
       </c>
       <c r="G23" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8345,22 +8561,22 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>527</v>
+        <v>554</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>528</v>
+        <v>555</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>529</v>
+        <v>556</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>530</v>
+        <v>557</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>531</v>
+        <v>558</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -8372,7 +8588,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>532</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8380,34 +8596,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>533</v>
+        <v>560</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>534</v>
+        <v>561</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>535</v>
+        <v>562</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>537</v>
+        <v>564</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>539</v>
+        <v>566</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>540</v>
+        <v>567</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>541</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8415,34 +8631,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>533</v>
+        <v>560</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>534</v>
+        <v>561</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>543</v>
+        <v>570</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>544</v>
+        <v>571</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>545</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8450,34 +8666,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>533</v>
+        <v>560</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>534</v>
+        <v>561</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>546</v>
+        <v>573</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>547</v>
+        <v>574</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>549</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8485,34 +8701,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>533</v>
+        <v>560</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>534</v>
+        <v>561</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>550</v>
+        <v>577</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>551</v>
+        <v>578</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>552</v>
+        <v>579</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>553</v>
+        <v>580</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8520,34 +8736,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>556</v>
+        <v>583</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>557</v>
+        <v>584</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>558</v>
+        <v>585</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>559</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8555,34 +8771,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>560</v>
+        <v>587</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>561</v>
+        <v>588</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>562</v>
+        <v>589</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>563</v>
+        <v>590</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8590,34 +8806,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>564</v>
+        <v>591</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>565</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>538</v>
-      </c>
       <c r="H8" s="0" t="s">
-        <v>566</v>
+        <v>593</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>567</v>
+        <v>594</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>568</v>
+        <v>595</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8625,34 +8841,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>569</v>
+        <v>596</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>570</v>
+        <v>597</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>571</v>
+        <v>598</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>572</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8660,34 +8876,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>573</v>
+        <v>600</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>574</v>
+        <v>601</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>575</v>
+        <v>602</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>576</v>
+        <v>603</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>577</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8695,34 +8911,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>573</v>
+        <v>600</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>578</v>
+        <v>605</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>503</v>
+        <v>516</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>579</v>
+        <v>517</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>580</v>
+        <v>606</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>581</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8730,34 +8946,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>573</v>
+        <v>600</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>582</v>
+        <v>608</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>583</v>
+        <v>609</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>584</v>
+        <v>610</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>585</v>
+        <v>611</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8765,34 +8981,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>554</v>
+        <v>581</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>586</v>
+        <v>612</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>587</v>
+        <v>613</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>588</v>
+        <v>614</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>589</v>
+        <v>615</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>590</v>
+        <v>616</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8800,34 +9016,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>592</v>
+        <v>618</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>458</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>593</v>
+        <v>619</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>594</v>
+        <v>531</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>595</v>
+        <v>620</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8835,34 +9051,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>592</v>
+        <v>618</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>596</v>
+        <v>621</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>597</v>
+        <v>622</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>598</v>
+        <v>623</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>599</v>
+        <v>624</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8870,34 +9086,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>533</v>
+        <v>560</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>535</v>
+        <v>562</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>592</v>
+        <v>618</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>600</v>
+        <v>625</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>601</v>
+        <v>626</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>602</v>
+        <v>627</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>603</v>
+        <v>628</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8905,34 +9121,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>604</v>
+        <v>629</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>605</v>
+        <v>630</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>606</v>
+        <v>631</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>607</v>
+        <v>632</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>608</v>
+        <v>633</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8940,34 +9156,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>609</v>
+        <v>634</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>610</v>
+        <v>635</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>415</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>612</v>
+        <v>637</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8975,34 +9191,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>613</v>
+        <v>638</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>586</v>
+        <v>612</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>614</v>
+        <v>639</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>615</v>
+        <v>640</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>616</v>
+        <v>641</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>617</v>
+        <v>642</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>483</v>
+        <v>643</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>618</v>
+        <v>644</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9010,34 +9226,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>521</v>
+        <v>544</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>522</v>
+        <v>546</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>620</v>
+        <v>547</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>523</v>
+        <v>646</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>621</v>
+        <v>647</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9045,34 +9261,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>555</v>
+        <v>582</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>526</v>
+        <v>552</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>622</v>
+        <v>553</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>623</v>
+        <v>648</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>624</v>
+        <v>649</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added table for indicators computed from output variables
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -42,13 +42,15 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="651">
   <si>
     <t>name.rsunflo.fr</t>
   </si>
@@ -461,7 +463,7 @@
     <t>field_capacity_1</t>
   </si>
   <si>
-    <t>WaterCapacity</t>
+    <t>SoilWaterCapacity</t>
   </si>
   <si>
     <t>Humidité massique à la capacité au champ dans l'horizon de surface (0 - 30 cm)</t>
@@ -1457,6 +1459,9 @@
     <t>Température minimale</t>
   </si>
   <si>
+    <t>$°C$</t>
+  </si>
+  <si>
     <t>Tx</t>
   </si>
   <si>
@@ -1481,12 +1486,15 @@
     <t>RG</t>
   </si>
   <si>
-    <t>MJ/m2</t>
+    <t>$MJ.m^{-2}$</t>
   </si>
   <si>
     <t>ETPP</t>
   </si>
   <si>
+    <t>$mm$</t>
+  </si>
+  <si>
     <t>Pluie</t>
   </si>
   <si>
@@ -1508,6 +1516,9 @@
     <t>Temperature sum from emergence</t>
   </si>
   <si>
+    <t>$°C.d$</t>
+  </si>
+  <si>
     <t>PhasePhenoPlante</t>
   </si>
   <si>
@@ -1517,7 +1528,7 @@
     <t>Index de phénologie</t>
   </si>
   <si>
-    <t>Phenological stages index </t>
+    <t>Phenological stages index</t>
   </si>
   <si>
     <t>contrainte_eau</t>
@@ -1604,7 +1615,7 @@
     <t>Absorbed nitrogen</t>
   </si>
   <si>
-    <t>kg.ha-1.d-1</t>
+    <t>$kg.ha^{-1}.d^{-1}$</t>
   </si>
   <si>
     <t>INN</t>
@@ -1673,7 +1684,7 @@
     <t>Crop aerial dry biomass</t>
   </si>
   <si>
-    <t>g.m-2</t>
+    <t>$g.m^{-2}$</t>
   </si>
   <si>
     <t>elaboration_rendement</t>
@@ -1694,7 +1705,7 @@
     <t>Grain yield</t>
   </si>
   <si>
-    <t>q.ha-1</t>
+    <t>$q.ha^{-1}$</t>
   </si>
   <si>
     <t>elaboration_qualite</t>
@@ -1712,6 +1723,9 @@
     <t>Grain oil content</t>
   </si>
   <si>
+    <t>$\% (dry matter)$</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
@@ -1754,7 +1768,7 @@
     <t>Photosynthetically active radiation</t>
   </si>
   <si>
-    <t>sum(GR*0.48)</t>
+    <t>$sum(GR*0.48)$</t>
   </si>
   <si>
     <t>water</t>
@@ -1766,7 +1780,7 @@
     <t>Rain</t>
   </si>
   <si>
-    <t>sum(RR)</t>
+    <t>$sum(RR)$</t>
   </si>
   <si>
     <t>SETP</t>
@@ -1778,7 +1792,7 @@
     <t>Potential evapotranspiration</t>
   </si>
   <si>
-    <t>sum(ETP)</t>
+    <t>$sum(ETP)$</t>
   </si>
   <si>
     <t>SCWD</t>
@@ -1790,7 +1804,7 @@
     <t>Climatic water deficit</t>
   </si>
   <si>
-    <t>sum(P-ETP)</t>
+    <t>$sum(P-ETP)$</t>
   </si>
   <si>
     <t>constraint</t>
@@ -1808,7 +1822,7 @@
     <t>Edaphic water deficit (continuous)</t>
   </si>
   <si>
-    <t>sum(1-FTSW)</t>
+    <t>$sum(1-FTSW)$</t>
   </si>
   <si>
     <t>NETR</t>
@@ -1820,7 +1834,7 @@
     <t>Edaphic water deficit (discrete)</t>
   </si>
   <si>
-    <t>sum(ETR/ETM &lt; 0.6)</t>
+    <t>$sum(ETR/ETM &lt; 0.6)$</t>
   </si>
   <si>
     <t>transpiration</t>
@@ -1835,7 +1849,7 @@
     <t>Water stress impact on crop transpiration</t>
   </si>
   <si>
-    <t>sum(1-FHTR)</t>
+    <t>$sum(1-FHTR)$</t>
   </si>
   <si>
     <t>SFHRUE</t>
@@ -1847,7 +1861,7 @@
     <t>Water stress impact on crop photosynthesis</t>
   </si>
   <si>
-    <t>sum(1-FHRUE)</t>
+    <t>$sum(1-FHRUE)$</t>
   </si>
   <si>
     <t>nitrogen</t>
@@ -1862,16 +1876,16 @@
     <t>Nitrogen deficit</t>
   </si>
   <si>
-    <t>sum(1-NNI)</t>
+    <t>$sum(1-NNI)$</t>
   </si>
   <si>
     <t>SNAB</t>
   </si>
   <si>
-    <t>kg/ha</t>
-  </si>
-  <si>
-    <t>diff(range(NAB))</t>
+    <t>$kg.ha^{-1}$</t>
+  </si>
+  <si>
+    <t>$diff(range(NAB))$</t>
   </si>
   <si>
     <t>SFNRUE</t>
@@ -1883,7 +1897,7 @@
     <t>Nitrogen stress impact on photosynthesis</t>
   </si>
   <si>
-    <t>sum(1-FNRUE)</t>
+    <t>$sum(1-FNRUE)$</t>
   </si>
   <si>
     <t>temperature</t>
@@ -1898,7 +1912,7 @@
     <t>Thermal stress impact on photosynthesis</t>
   </si>
   <si>
-    <t>sum(1-FTRUE)</t>
+    <t>$sum(1-FTRUE)$</t>
   </si>
   <si>
     <t>state</t>
@@ -1910,7 +1924,7 @@
     <t>Indice foliaire maximum</t>
   </si>
   <si>
-    <t>max(LAI)</t>
+    <t>$max(LAI)$</t>
   </si>
   <si>
     <t>DSF</t>
@@ -1922,7 +1936,7 @@
     <t>Leaf area duration</t>
   </si>
   <si>
-    <t>sum(LAI)</t>
+    <t>$sum(LAI)$</t>
   </si>
   <si>
     <t>SIR</t>
@@ -1934,7 +1948,7 @@
     <t>Intercepted radiation</t>
   </si>
   <si>
-    <t>sum(RIE*GR*0.48)</t>
+    <t>$sum(RIE*GR*0.48)$</t>
   </si>
   <si>
     <t>MRUE</t>
@@ -1946,10 +1960,10 @@
     <t>Photosynthesis</t>
   </si>
   <si>
-    <t>g/MJ/m2</t>
-  </si>
-  <si>
-    <t>mean(RUE)</t>
+    <t>$g.MJ^{-1}.m^{-2}$</t>
+  </si>
+  <si>
+    <t>$mean(RUE)$</t>
   </si>
   <si>
     <t>STDM</t>
@@ -1961,7 +1975,7 @@
     <t>Aerial Biomass</t>
   </si>
   <si>
-    <t>max(TDM)</t>
+    <t>$max(TDM)$</t>
   </si>
   <si>
     <t>ressource</t>
@@ -1979,25 +1993,16 @@
     <t>Thermal time</t>
   </si>
   <si>
-    <t>°C.j</t>
-  </si>
-  <si>
-    <t>max(TTA2)</t>
+    <t>$max(TTA2)$</t>
   </si>
   <si>
     <t>performance</t>
   </si>
   <si>
-    <t>q/ha</t>
-  </si>
-  <si>
-    <t>max(GY)</t>
-  </si>
-  <si>
-    <t>% (DM)</t>
-  </si>
-  <si>
-    <t>max(OC)</t>
+    <t>$max(GY)$</t>
+  </si>
+  <si>
+    <t>$max(OC)$</t>
   </si>
 </sst>
 </file>
@@ -2144,7 +2149,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="I22 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -2278,7 +2283,7 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="1" sqref="I22 J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -7606,7 +7611,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="I22 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -7766,7 +7771,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -7841,7 +7846,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>9</v>
+        <v>469</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
@@ -7858,7 +7863,7 @@
         <v>466</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
@@ -7867,13 +7872,13 @@
         <v>11</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>9</v>
+        <v>469</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>1</v>
@@ -7890,22 +7895,22 @@
         <v>466</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>9</v>
+        <v>469</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>1</v>
@@ -7922,7 +7927,7 @@
         <v>466</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -7937,7 +7942,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>1</v>
@@ -7954,7 +7959,7 @@
         <v>466</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
@@ -7969,7 +7974,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>23</v>
+        <v>480</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>1</v>
@@ -7986,7 +7991,7 @@
         <v>466</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -8001,7 +8006,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>23</v>
+        <v>480</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>1</v>
@@ -8012,28 +8017,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>449</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>52</v>
+        <v>488</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>1</v>
@@ -8044,25 +8049,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>91</v>
@@ -8076,25 +8081,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>91</v>
@@ -8108,25 +8113,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>91</v>
@@ -8140,25 +8145,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>496</v>
-      </c>
       <c r="G12" s="0" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>91</v>
@@ -8172,25 +8177,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>91</v>
@@ -8204,25 +8209,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>91</v>
@@ -8236,28 +8241,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>1</v>
@@ -8268,25 +8273,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>91</v>
@@ -8300,25 +8305,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>91</v>
@@ -8332,10 +8337,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>458</v>
@@ -8347,10 +8352,10 @@
         <v>458</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>91</v>
@@ -8364,13 +8369,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>459</v>
@@ -8379,10 +8384,10 @@
         <v>459</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>91</v>
@@ -8396,13 +8401,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>461</v>
@@ -8411,10 +8416,10 @@
         <v>461</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>91</v>
@@ -8428,28 +8433,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>460</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>1</v>
@@ -8460,28 +8465,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>1</v>
@@ -8492,28 +8497,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>114</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>118</v>
+        <v>557</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>1</v>
@@ -8536,10 +8541,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="1" sqref="I22 J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.2"/>
@@ -8556,27 +8561,27 @@
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -8588,637 +8593,637 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>23</v>
+        <v>480</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>23</v>
+        <v>480</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>23</v>
+        <v>480</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>569</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>591</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>592</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>565</v>
-      </c>
       <c r="H8" s="0" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>567</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>569</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>565</v>
-      </c>
       <c r="H9" s="0" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>458</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>415</v>
+        <v>544</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>643</v>
+        <v>488</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9226,72 +9231,71 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>646</v>
+        <v>551</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>648</v>
+        <v>557</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>650</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
modified rsunflo::indicate to include a high/low thermal stress indicator
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="233" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="233" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,13 +44,15 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="647">
   <si>
     <t>name.rsunflo.fr</t>
   </si>
@@ -208,7 +210,7 @@
     <t>Temperature sum to floral initiation</t>
   </si>
   <si>
-    <t>°Cd</t>
+    <t>$°C.d$</t>
   </si>
   <si>
     <t>[@Lecoeur2011]</t>
@@ -274,7 +276,7 @@
     <t>Potential number of leaves at flowering</t>
   </si>
   <si>
-    <t>leaf</t>
+    <t>$leaf$</t>
   </si>
   <si>
     <t>bSF</t>
@@ -286,7 +288,7 @@
     <t>PotentialLeafProfile</t>
   </si>
   <si>
-    <t>Rang (depuis le sol) de la plus grande feuille du profil foliaire à la floraison</t>
+    <t>Rang de la plus grande feuille du profil à la floraison</t>
   </si>
   <si>
     <t>Potential rank of the plant largest leaf at flowering</t>
@@ -301,13 +303,13 @@
     <t>PotentialLeafSize</t>
   </si>
   <si>
-    <t>Surface de la plus grande feuille du profil folaire à la floraison</t>
+    <t>Surface de la plus grande feuille du profil à la floraison</t>
   </si>
   <si>
     <t>Potential area of the plant largest leaf at flowering</t>
   </si>
   <si>
-    <t>cm2</t>
+    <t>$cm^{-2}$</t>
   </si>
   <si>
     <t>ext</t>
@@ -406,7 +408,7 @@
     <t>Potential seed oil content</t>
   </si>
   <si>
-    <t>% dry matter</t>
+    <t>$\% dry_matter$</t>
   </si>
   <si>
     <t>Pedoclimat</t>
@@ -454,6 +456,9 @@
     <t>Potential rooting depth</t>
   </si>
   <si>
+    <t>$mm$</t>
+  </si>
+  <si>
     <t>Hcc_C1</t>
   </si>
   <si>
@@ -472,7 +477,7 @@
     <t>Water content at field capacity (0-30 cm)</t>
   </si>
   <si>
-    <t>%</t>
+    <t>$\%$</t>
   </si>
   <si>
     <t>Hpf_C1</t>
@@ -538,7 +543,7 @@
     <t>Soil bulk density (0-30cm)</t>
   </si>
   <si>
-    <t>g.cm-3</t>
+    <t>$g.cm^{-3}$</t>
   </si>
   <si>
     <t>da_C2</t>
@@ -574,7 +579,7 @@
     <t>Stone content (0-rooting depth)</t>
   </si>
   <si>
-    <t>[0 ; 1]</t>
+    <t>$[0,1]$</t>
   </si>
   <si>
     <t>Vp</t>
@@ -595,7 +600,7 @@
     <t>Potential nitrogen mineralization rate</t>
   </si>
   <si>
-    <t>kg/ha/day (normalized)</t>
+    <t>$kg.ha^{-1}.day^{-1} (normalized)$</t>
   </si>
   <si>
     <t>[@Vale2007]</t>
@@ -634,7 +639,7 @@
     <t>Sowing date</t>
   </si>
   <si>
-    <t>dd/mm</t>
+    <t>$date (dd/mm)$</t>
   </si>
   <si>
     <t>jrecolte</t>
@@ -688,7 +693,7 @@
     <t>Plant density</t>
   </si>
   <si>
-    <t>pnt/m2</t>
+    <t>$plant.m^{-2}$</t>
   </si>
   <si>
     <t>date_ferti_1</t>
@@ -724,7 +729,7 @@
     <t>Fertilization (amount 1)</t>
   </si>
   <si>
-    <t>kg/ha eq. mineral nitrogen</t>
+    <t>$kg.ha^{-1}$ eq. mineral nitrogen</t>
   </si>
   <si>
     <t>date_ferti_2</t>
@@ -994,7 +999,7 @@
     <t>Date de début de la simulation</t>
   </si>
   <si>
-    <t>jj/mm/aaaa</t>
+    <t>$date (dd/mm/aaaa)$</t>
   </si>
   <si>
     <t>duration</t>
@@ -1003,7 +1008,7 @@
     <t>Durée de la simulation</t>
   </si>
   <si>
-    <t>jour</t>
+    <t>$day$</t>
   </si>
   <si>
     <t>CONFIG_SimuInit</t>
@@ -1021,9 +1026,6 @@
     <t>Date de levée forcée, simulée pour valeur = 01/01</t>
   </si>
   <si>
-    <t>jj/mm</t>
-  </si>
-  <si>
     <t>rh1</t>
   </si>
   <si>
@@ -1093,6 +1095,9 @@
     <t>Température de base pour les processus de croissance et développement</t>
   </si>
   <si>
+    <t>$°C$</t>
+  </si>
+  <si>
     <t>[@Granier1998]</t>
   </si>
   <si>
@@ -1204,7 +1209,7 @@
     <t>Valeur initiale (0-300°Cj) de l'efficience biologique potentielle</t>
   </si>
   <si>
-    <t>g/m2/MJ</t>
+    <t>$g.MJ^{-1}.m^{-2}$</t>
   </si>
   <si>
     <t>Eb_c</t>
@@ -1297,7 +1302,7 @@
     <t>Seuil de biomasse aerienne au stade juvénile considéré pour la courbe de dilution d'azote critique</t>
   </si>
   <si>
-    <t>g/m2</t>
+    <t>$g.m^{-2}$</t>
   </si>
   <si>
     <t>TDMm_seuil</t>
@@ -1327,7 +1332,7 @@
     <t>Vitesse de croissance racinaire</t>
   </si>
   <si>
-    <t>mm/°Cd</t>
+    <t>$mm.Cd{^-1}$</t>
   </si>
   <si>
     <t>EXPERT_SimuInit</t>
@@ -1357,7 +1362,7 @@
     <t>Reciprocal of hypocotyl elongation rate</t>
   </si>
   <si>
-    <t>°Cd/mm</t>
+    <t>$°Cd.mm^{-1}$</t>
   </si>
   <si>
     <t>[@Villalobos1996]</t>
@@ -1459,9 +1464,6 @@
     <t>Température minimale</t>
   </si>
   <si>
-    <t>$°C$</t>
-  </si>
-  <si>
     <t>Tx</t>
   </si>
   <si>
@@ -1492,9 +1494,6 @@
     <t>ETPP</t>
   </si>
   <si>
-    <t>$mm$</t>
-  </si>
-  <si>
     <t>Pluie</t>
   </si>
   <si>
@@ -1516,9 +1515,6 @@
     <t>Temperature sum from emergence</t>
   </si>
   <si>
-    <t>$°C.d$</t>
-  </si>
-  <si>
     <t>PhasePhenoPlante</t>
   </si>
   <si>
@@ -1684,9 +1680,6 @@
     <t>Crop aerial dry biomass</t>
   </si>
   <si>
-    <t>$g.m^{-2}$</t>
-  </si>
-  <si>
     <t>elaboration_rendement</t>
   </si>
   <si>
@@ -1958,9 +1951,6 @@
   </si>
   <si>
     <t>Photosynthesis</t>
-  </si>
-  <si>
-    <t>$g.MJ^{-1}.m^{-2}$</t>
   </si>
   <si>
     <t>$mean(RUE)$</t>
@@ -2149,7 +2139,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="I22 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -2282,8 +2272,8 @@
   </sheetPr>
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="1" sqref="I22 J20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -3046,7 +3036,9 @@
       <c r="L12" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="M12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="N12" s="0" t="s">
         <v>53</v>
       </c>
@@ -3281,7 +3273,7 @@
         <v>133</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="N16" s="0" t="s">
         <v>53</v>
@@ -3322,25 +3314,25 @@
         <v>128</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O17" s="0" t="n">
         <v>19.69</v>
@@ -3378,25 +3370,25 @@
         <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="O18" s="0" t="n">
         <v>9.69</v>
@@ -3434,25 +3426,25 @@
         <v>128</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O19" s="0" t="n">
         <v>19.69</v>
@@ -3490,25 +3482,25 @@
         <v>128</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O20" s="0" t="n">
         <v>9.69</v>
@@ -3546,25 +3538,25 @@
         <v>128</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="O21" s="0" t="n">
         <v>1.3</v>
@@ -3602,25 +3594,25 @@
         <v>128</v>
       </c>
       <c r="G22" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="O22" s="0" t="n">
         <v>1.3</v>
@@ -3658,25 +3650,25 @@
         <v>128</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O23" s="0" t="n">
         <v>0.1</v>
@@ -3714,28 +3706,28 @@
         <v>128</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O24" s="0" t="n">
         <v>0.5</v>
@@ -3773,16 +3765,16 @@
         <v>128</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O25" s="0" t="n">
         <v>0.2</v>
@@ -3811,34 +3803,34 @@
         <v>25</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O26" s="5" t="n">
         <v>41380</v>
@@ -3867,34 +3859,34 @@
         <v>26</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G27" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="O27" s="5" t="n">
         <v>41548</v>
@@ -3923,37 +3915,37 @@
         <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>46</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O28" s="4" t="n">
         <v>30</v>
@@ -3982,34 +3974,34 @@
         <v>28</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O29" s="4" t="n">
         <v>7</v>
@@ -4038,34 +4030,34 @@
         <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O30" s="6" t="n">
         <v>41275</v>
@@ -4094,34 +4086,34 @@
         <v>30</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O31" s="4" t="n">
         <v>0</v>
@@ -4150,34 +4142,34 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O32" s="6" t="n">
         <v>41275</v>
@@ -4206,34 +4198,34 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O33" s="4" t="n">
         <v>0</v>
@@ -4262,34 +4254,34 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O34" s="6" t="n">
         <v>41275</v>
@@ -4318,34 +4310,34 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O35" s="4" t="n">
         <v>0</v>
@@ -4374,34 +4366,34 @@
         <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O36" s="6" t="n">
         <v>41275</v>
@@ -4430,34 +4422,34 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O37" s="4" t="n">
         <v>0</v>
@@ -4486,34 +4478,34 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O38" s="6" t="n">
         <v>41275</v>
@@ -4542,34 +4534,34 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O39" s="4" t="n">
         <v>0</v>
@@ -4598,34 +4590,34 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O40" s="6" t="n">
         <v>41275</v>
@@ -4654,34 +4646,34 @@
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O41" s="4" t="n">
         <v>0</v>
@@ -4710,34 +4702,34 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O42" s="6" t="n">
         <v>41275</v>
@@ -4766,34 +4758,34 @@
         <v>42</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O43" s="4" t="n">
         <v>0</v>
@@ -4822,34 +4814,34 @@
         <v>43</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O44" s="6" t="n">
         <v>41275</v>
@@ -4878,34 +4870,34 @@
         <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O45" s="4" t="n">
         <v>0</v>
@@ -4934,34 +4926,34 @@
         <v>45</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L46" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O46" s="6" t="n">
         <v>41275</v>
@@ -4990,34 +4982,34 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O47" s="4" t="n">
         <v>0</v>
@@ -5046,34 +5038,34 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L48" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O48" s="6" t="n">
         <v>41275</v>
@@ -5102,34 +5094,34 @@
         <v>48</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L49" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O49" s="4" t="n">
         <v>0</v>
@@ -5158,25 +5150,25 @@
         <v>49</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O50" s="5" t="n">
         <v>41373</v>
@@ -5205,25 +5197,25 @@
         <v>50</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M51" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="O51" s="0" t="n">
         <v>180</v>
@@ -5252,28 +5244,28 @@
         <v>51</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>323</v>
+        <v>195</v>
       </c>
       <c r="O52" s="6" t="n">
         <v>41275</v>
@@ -5302,13 +5294,13 @@
         <v>52</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>324</v>
@@ -5323,7 +5315,7 @@
         <v>327</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O53" s="0" t="n">
         <v>10</v>
@@ -5352,13 +5344,13 @@
         <v>53</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>328</v>
@@ -5373,7 +5365,7 @@
         <v>331</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O54" s="0" t="n">
         <v>20</v>
@@ -5402,13 +5394,13 @@
         <v>54</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>332</v>
@@ -5423,7 +5415,7 @@
         <v>335</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O55" s="0" t="n">
         <v>19.7</v>
@@ -5452,13 +5444,13 @@
         <v>55</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G56" s="0" t="s">
         <v>336</v>
@@ -5473,7 +5465,7 @@
         <v>339</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O56" s="0" t="n">
         <v>19.7</v>
@@ -5502,13 +5494,13 @@
         <v>56</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G57" s="0" t="s">
         <v>340</v>
@@ -5517,7 +5509,7 @@
         <v>341</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="O57" s="4" t="n">
         <v>300</v>
@@ -5561,10 +5553,10 @@
         <v>346</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O58" s="4" t="n">
         <v>4.8</v>
@@ -5605,16 +5597,16 @@
         <v>46</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>52</v>
@@ -5661,22 +5653,22 @@
         <v>69</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N60" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O60" s="4" t="n">
         <v>71.43</v>
@@ -5717,22 +5709,22 @@
         <v>69</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L61" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M61" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N61" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O61" s="4" t="n">
         <v>16.34</v>
@@ -5770,16 +5762,16 @@
         <v>344</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K62" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="N62" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O62" s="4" t="n">
         <v>1800</v>
@@ -5817,16 +5809,16 @@
         <v>344</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M63" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N63" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O63" s="4" t="n">
         <v>0.1</v>
@@ -5864,16 +5856,16 @@
         <v>344</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M64" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N64" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O64" s="4" t="n">
         <v>400</v>
@@ -5911,16 +5903,16 @@
         <v>344</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="K65" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M65" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N65" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O65" s="4" t="n">
         <v>1</v>
@@ -5958,16 +5950,16 @@
         <v>344</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M66" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N66" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O66" s="4" t="n">
         <v>153</v>
@@ -6008,22 +6000,22 @@
         <v>69</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L67" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N67" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O67" s="4" t="n">
         <v>851.33</v>
@@ -6061,16 +6053,16 @@
         <v>344</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K68" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M68" s="3" t="s">
         <v>74</v>
       </c>
       <c r="N68" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O68" s="4" t="n">
         <v>-0.03783</v>
@@ -6108,16 +6100,16 @@
         <v>344</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="K69" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O69" s="4" t="n">
         <v>0.78469</v>
@@ -6155,16 +6147,16 @@
         <v>344</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="K70" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M70" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N70" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O70" s="4" t="n">
         <v>0.01379</v>
@@ -6202,13 +6194,13 @@
         <v>344</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="K71" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="M71" s="3" t="s">
         <v>384</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>385</v>
       </c>
       <c r="N71" s="0" t="s">
         <v>112</v>
@@ -6249,13 +6241,13 @@
         <v>344</v>
       </c>
       <c r="G72" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="K72" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="M72" s="0" t="s">
         <v>385</v>
-      </c>
-      <c r="K72" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="M72" s="3" t="s">
-        <v>384</v>
       </c>
       <c r="N72" s="0" t="s">
         <v>112</v>
@@ -6296,13 +6288,13 @@
         <v>344</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="K73" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="M73" s="3" t="s">
-        <v>384</v>
+        <v>389</v>
+      </c>
+      <c r="M73" s="0" t="s">
+        <v>385</v>
       </c>
       <c r="N73" s="0" t="s">
         <v>112</v>
@@ -6343,13 +6335,13 @@
         <v>344</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="K74" s="0" t="s">
-        <v>390</v>
-      </c>
-      <c r="M74" s="3" t="s">
-        <v>384</v>
+        <v>391</v>
+      </c>
+      <c r="M74" s="0" t="s">
+        <v>385</v>
       </c>
       <c r="N74" s="0" t="s">
         <v>112</v>
@@ -6390,13 +6382,13 @@
         <v>344</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K75" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="N75" s="0" t="s">
         <v>112</v>
@@ -6437,14 +6429,14 @@
         <v>344</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="L76" s="3"/>
       <c r="M76" s="3" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="N76" s="0" t="s">
         <v>112</v>
@@ -6485,14 +6477,14 @@
         <v>344</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L77" s="3"/>
       <c r="M77" s="3" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="N77" s="0" t="s">
         <v>112</v>
@@ -6533,16 +6525,16 @@
         <v>344</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="K78" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M78" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N78" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O78" s="4" t="n">
         <v>-25</v>
@@ -6580,16 +6572,16 @@
         <v>344</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>52</v>
+        <v>347</v>
       </c>
       <c r="N79" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O79" s="4" t="n">
         <v>350</v>
@@ -6627,16 +6619,16 @@
         <v>344</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="K80" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M80" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N80" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O80" s="4" t="n">
         <v>0.1</v>
@@ -6671,19 +6663,19 @@
         <v>343</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="K81" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N81" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O81" s="4" t="n">
         <v>4.53</v>
@@ -6718,19 +6710,19 @@
         <v>343</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="K82" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M82" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N82" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O82" s="4" t="n">
         <v>0.42</v>
@@ -6765,19 +6757,19 @@
         <v>343</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="K83" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N83" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O83" s="4" t="n">
         <v>6.49</v>
@@ -6812,19 +6804,19 @@
         <v>343</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K84" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M84" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N84" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O84" s="4" t="n">
         <v>0.44</v>
@@ -6859,19 +6851,19 @@
         <v>343</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="K85" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="M85" s="3" t="s">
         <v>415</v>
       </c>
+      <c r="M85" s="0" t="s">
+        <v>416</v>
+      </c>
       <c r="N85" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O85" s="4" t="n">
         <v>75</v>
@@ -6906,19 +6898,19 @@
         <v>343</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G86" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="K86" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="M86" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="K86" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="M86" s="3" t="s">
-        <v>415</v>
-      </c>
       <c r="N86" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O86" s="4" t="n">
         <v>75</v>
@@ -6953,19 +6945,19 @@
         <v>343</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K87" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M87" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N87" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="O87" s="4" t="n">
         <v>0.6</v>
@@ -7000,19 +6992,19 @@
         <v>343</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="K88" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M88" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N88" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="O88" s="4" t="n">
         <v>0.3</v>
@@ -7047,16 +7039,16 @@
         <v>343</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="K89" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="N89" s="0" t="s">
         <v>53</v>
@@ -7094,13 +7086,13 @@
         <v>343</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="K90" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M90" s="3" t="s">
         <v>91</v>
@@ -7138,13 +7130,13 @@
         <v>343</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K91" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M91" s="3" t="s">
         <v>91</v>
@@ -7185,28 +7177,28 @@
         <v>343</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>46</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="K92" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L92" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="N92" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O92" s="4" t="n">
         <v>1.19</v>
@@ -7235,16 +7227,16 @@
         <v>100</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="M93" s="3"/>
       <c r="P93" s="0" t="n">
@@ -7271,16 +7263,16 @@
         <v>101</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="M94" s="3"/>
       <c r="P94" s="0" t="n">
@@ -7307,16 +7299,16 @@
         <v>102</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="M95" s="3"/>
       <c r="P95" s="0" t="n">
@@ -7343,16 +7335,16 @@
         <v>103</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M96" s="3"/>
       <c r="P96" s="0" t="n">
@@ -7379,16 +7371,16 @@
         <v>104</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="M97" s="3"/>
       <c r="P97" s="0" t="n">
@@ -7415,16 +7407,16 @@
         <v>105</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M98" s="3"/>
       <c r="P98" s="0" t="n">
@@ -7451,16 +7443,16 @@
         <v>106</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="M99" s="3"/>
       <c r="P99" s="0" t="n">
@@ -7487,16 +7479,16 @@
         <v>107</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="M100" s="3"/>
       <c r="P100" s="0" t="n">
@@ -7523,16 +7515,16 @@
         <v>108</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="M101" s="3"/>
       <c r="P101" s="0" t="n">
@@ -7559,16 +7551,16 @@
         <v>109</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="P102" s="0" t="n">
         <v>0</v>
@@ -7611,7 +7603,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="I22 A23"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -7652,7 +7644,7 @@
         <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7660,7 +7652,7 @@
         <v>69</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7668,7 +7660,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7676,7 +7668,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7684,7 +7676,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7692,7 +7684,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7700,7 +7692,7 @@
         <v>69</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7713,42 +7705,42 @@
     </row>
     <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -7770,7 +7762,7 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -7793,10 +7785,10 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -7817,7 +7809,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7825,13 +7817,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -7840,13 +7832,13 @@
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>469</v>
+        <v>347</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
@@ -7857,10 +7849,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>470</v>
@@ -7878,7 +7870,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>469</v>
+        <v>347</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>1</v>
@@ -7889,10 +7881,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>472</v>
@@ -7910,7 +7902,7 @@
         <v>476</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>469</v>
+        <v>347</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>1</v>
@@ -7921,10 +7913,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>477</v>
@@ -7953,10 +7945,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>479</v>
@@ -7974,7 +7966,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>480</v>
+        <v>134</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>1</v>
@@ -7985,13 +7977,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -8006,7 +7998,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>480</v>
+        <v>134</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>1</v>
@@ -8017,28 +8009,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>486</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>487</v>
-      </c>
       <c r="I8" s="0" t="s">
-        <v>488</v>
+        <v>52</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>1</v>
@@ -8049,25 +8041,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>483</v>
-      </c>
       <c r="D9" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>489</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="H9" s="0" t="s">
         <v>490</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>492</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>91</v>
@@ -8081,25 +8073,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="G10" s="0" t="s">
         <v>494</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="H10" s="0" t="s">
         <v>495</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>497</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>91</v>
@@ -8113,25 +8105,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="H11" s="0" t="s">
         <v>499</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>501</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>91</v>
@@ -8145,25 +8137,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>502</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>504</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>91</v>
@@ -8177,25 +8169,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="H13" s="0" t="s">
         <v>506</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>507</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>508</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>91</v>
@@ -8209,25 +8201,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="G14" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="H14" s="0" t="s">
         <v>512</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>514</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>91</v>
@@ -8241,28 +8233,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="G15" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="H15" s="0" t="s">
         <v>518</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>519</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>520</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>521</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>1</v>
@@ -8273,25 +8265,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="G16" s="0" t="s">
         <v>523</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="H16" s="0" t="s">
         <v>524</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>526</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>91</v>
@@ -8305,25 +8297,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="G17" s="0" t="s">
         <v>528</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="H17" s="0" t="s">
         <v>529</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>531</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>91</v>
@@ -8337,25 +8329,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>532</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>533</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>534</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>91</v>
@@ -8369,25 +8361,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>535</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>536</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>537</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>91</v>
@@ -8401,25 +8393,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="H20" s="0" t="s">
         <v>538</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>540</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>91</v>
@@ -8433,28 +8425,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="H21" s="0" t="s">
         <v>541</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>543</v>
-      </c>
       <c r="I21" s="0" t="s">
-        <v>544</v>
+        <v>416</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>1</v>
@@ -8465,28 +8457,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="G22" s="0" t="s">
         <v>546</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="H22" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="I22" s="0" t="s">
         <v>548</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>549</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>550</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>551</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>1</v>
@@ -8497,28 +8489,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>114</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>554</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>555</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>556</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>557</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>1</v>
@@ -8544,7 +8536,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="1" sqref="I22 J20"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.2"/>
@@ -8566,22 +8558,22 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>561</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -8593,7 +8585,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8601,34 +8593,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>565</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>567</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>568</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>570</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>571</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>478</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8636,34 +8628,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>480</v>
+        <v>134</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8671,34 +8663,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>575</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>576</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>577</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>579</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8706,34 +8698,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>578</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>581</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8741,34 +8733,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8776,34 +8768,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8811,34 +8803,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>595</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>598</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8846,34 +8838,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8881,34 +8873,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8916,34 +8908,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8951,34 +8943,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8986,34 +8978,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>613</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>616</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>617</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>618</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>619</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9021,34 +9013,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9056,34 +9048,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>622</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>625</v>
-      </c>
       <c r="G15" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9091,34 +9083,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>629</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>569</v>
-      </c>
       <c r="H16" s="0" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>478</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9126,34 +9118,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>630</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>631</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>633</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>634</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>635</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>636</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9161,34 +9153,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>544</v>
+        <v>416</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9196,34 +9188,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>613</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>642</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>586</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>616</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="J19" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="0" t="s">
         <v>643</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>644</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>645</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>646</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9231,34 +9223,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>549</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>550</v>
-      </c>
       <c r="J20" s="0" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9266,34 +9258,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified rsunflo::indicate to use similar names in crop (default) or phase (diagvar) outputs.
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="233" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="248" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,13 +46,17 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$Q$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="723">
   <si>
     <t>name.rsunflo.fr</t>
   </si>
@@ -1719,6 +1723,9 @@
     <t>$\% (dry matter)$</t>
   </si>
   <si>
+    <t>verbose</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
@@ -1731,12 +1738,15 @@
     <t>process</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>formula</t>
   </si>
   <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
     <t>resource</t>
   </si>
   <si>
@@ -1752,9 +1762,6 @@
     <t>SGR</t>
   </si>
   <si>
-    <t>cycle</t>
-  </si>
-  <si>
     <t>Rayonnement incident (PAR)</t>
   </si>
   <si>
@@ -1785,7 +1792,7 @@
     <t>Potential evapotranspiration</t>
   </si>
   <si>
-    <t>$sum(ETP)$</t>
+    <t>$sum(PET)$</t>
   </si>
   <si>
     <t>SCWD</t>
@@ -1797,13 +1804,115 @@
     <t>Climatic water deficit</t>
   </si>
   <si>
-    <t>$sum(P-ETP)$</t>
+    <t>$sum(RR-PET)$</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>phenology</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Temps thermique (base 4.8°C)</t>
+  </si>
+  <si>
+    <t>Thermal time (4.8 C basis)</t>
+  </si>
+  <si>
+    <t>$sum(TM - 4.8)$</t>
+  </si>
+  <si>
+    <t>D_SE</t>
+  </si>
+  <si>
+    <t>Durée de la phase semis - levée</t>
+  </si>
+  <si>
+    <t>Duration of sowing - emergence phase</t>
+  </si>
+  <si>
+    <t>$d$</t>
+  </si>
+  <si>
+    <t>emergence</t>
+  </si>
+  <si>
+    <t>D_EF</t>
+  </si>
+  <si>
+    <t>Durée de la phase végétative</t>
+  </si>
+  <si>
+    <t>Duration of vegetative phase</t>
+  </si>
+  <si>
+    <t>vegetative</t>
+  </si>
+  <si>
+    <t>D_FM</t>
+  </si>
+  <si>
+    <t>Durée de la phase de floraison</t>
+  </si>
+  <si>
+    <t>Duration of flowering phase</t>
+  </si>
+  <si>
+    <t>flowering</t>
+  </si>
+  <si>
+    <t>D_MH</t>
+  </si>
+  <si>
+    <t>Durée de la phase de remplissage</t>
+  </si>
+  <si>
+    <t>Duration of grain filling phase</t>
+  </si>
+  <si>
+    <t>filling</t>
   </si>
   <si>
     <t>constraint</t>
   </si>
   <si>
-    <t>crop</t>
+    <t>NHT</t>
+  </si>
+  <si>
+    <t>Nombre de jours de hautes tempértures</t>
+  </si>
+  <si>
+    <t>Thermal stress, high temperature (discrete)</t>
+  </si>
+  <si>
+    <t>$sum(TM &gt; 28)$</t>
+  </si>
+  <si>
+    <t>NLT</t>
+  </si>
+  <si>
+    <t>Nombre de jours de basses butes tempértures</t>
+  </si>
+  <si>
+    <t>Thermal stress, low temperature (discrete)</t>
+  </si>
+  <si>
+    <t>$sum(TM &lt; 20)$</t>
+  </si>
+  <si>
+    <t>SFTRUE</t>
+  </si>
+  <si>
+    <t>Effet de la contrainte thermique sur la photosynthèse</t>
+  </si>
+  <si>
+    <t>Thermal stress impact on photosynthesis</t>
+  </si>
+  <si>
+    <t>$sum(1-FTRUE)$</t>
   </si>
   <si>
     <t>SFTSW</t>
@@ -1827,7 +1936,7 @@
     <t>Edaphic water deficit (discrete)</t>
   </si>
   <si>
-    <t>$sum(ETR/ETM &lt; 0.6)$</t>
+    <t>$sum(ET/PET &lt; 0.6)$</t>
   </si>
   <si>
     <t>transpiration</t>
@@ -1863,10 +1972,10 @@
     <t>SNNI</t>
   </si>
   <si>
-    <t>Déficit azoté</t>
-  </si>
-  <si>
-    <t>Nitrogen deficit</t>
+    <t>Déficit azoté (continu)</t>
+  </si>
+  <si>
+    <t>Nitrogen deficit (continuous)</t>
   </si>
   <si>
     <t>$sum(1-NNI)$</t>
@@ -1893,21 +2002,6 @@
     <t>$sum(1-FNRUE)$</t>
   </si>
   <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>SFTRUE</t>
-  </si>
-  <si>
-    <t>Effet de la contrainte thermique sur la photosynthèse</t>
-  </si>
-  <si>
-    <t>Thermal stress impact on photosynthesis</t>
-  </si>
-  <si>
-    <t>$sum(1-FTRUE)$</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -1920,7 +2014,7 @@
     <t>$max(LAI)$</t>
   </si>
   <si>
-    <t>DSF</t>
+    <t>LAD</t>
   </si>
   <si>
     <t>Durée de surface foliaire</t>
@@ -1959,7 +2053,7 @@
     <t>STDM</t>
   </si>
   <si>
-    <t>Biomasse</t>
+    <t>Biomasse aerienne</t>
   </si>
   <si>
     <t>Aerial Biomass</t>
@@ -1968,24 +2062,6 @@
     <t>$max(TDM)$</t>
   </si>
   <si>
-    <t>ressource</t>
-  </si>
-  <si>
-    <t>phenology</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>Temps thermique (base 4.8°C)</t>
-  </si>
-  <si>
-    <t>Thermal time</t>
-  </si>
-  <si>
-    <t>$max(TTA2)$</t>
-  </si>
-  <si>
     <t>performance</t>
   </si>
   <si>
@@ -1993,6 +2069,162 @@
   </si>
   <si>
     <t>$max(OC)$</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>SGR_EF</t>
+  </si>
+  <si>
+    <t>SGR_FM</t>
+  </si>
+  <si>
+    <t>SGR_MH</t>
+  </si>
+  <si>
+    <t>SRR_EF</t>
+  </si>
+  <si>
+    <t>SRR_FM</t>
+  </si>
+  <si>
+    <t>SRR_MH</t>
+  </si>
+  <si>
+    <t>SCWD_EF</t>
+  </si>
+  <si>
+    <t>SCWD_FM</t>
+  </si>
+  <si>
+    <t>SCWD_MH</t>
+  </si>
+  <si>
+    <t>METR_EF</t>
+  </si>
+  <si>
+    <t>$mean(ET/PET)$</t>
+  </si>
+  <si>
+    <t>METR_FM</t>
+  </si>
+  <si>
+    <t>METR_FH</t>
+  </si>
+  <si>
+    <t>NETR_EF</t>
+  </si>
+  <si>
+    <t>NETR_FM</t>
+  </si>
+  <si>
+    <t>NETR_MH</t>
+  </si>
+  <si>
+    <t>SFTSW_EF</t>
+  </si>
+  <si>
+    <t>SFTSW_FM</t>
+  </si>
+  <si>
+    <t>SFTSW_MH</t>
+  </si>
+  <si>
+    <t>TT_SE</t>
+  </si>
+  <si>
+    <t>TT_EF</t>
+  </si>
+  <si>
+    <t>TT_FM</t>
+  </si>
+  <si>
+    <t>TT_MH</t>
+  </si>
+  <si>
+    <t>NLT_EF</t>
+  </si>
+  <si>
+    <t>Nombre de jours froids</t>
+  </si>
+  <si>
+    <t>Thermal stress, cold (discrete)</t>
+  </si>
+  <si>
+    <t>NLT_FM</t>
+  </si>
+  <si>
+    <t>NLT_MH</t>
+  </si>
+  <si>
+    <t>NHT_EF</t>
+  </si>
+  <si>
+    <t>Nombre de jours chauds</t>
+  </si>
+  <si>
+    <t>Thermal stress, heath (discrete)</t>
+  </si>
+  <si>
+    <t>NHT_FM</t>
+  </si>
+  <si>
+    <t>NHT_MH</t>
+  </si>
+  <si>
+    <t>SNAB_EM</t>
+  </si>
+  <si>
+    <t>Azote absorbé jusqu'à la fin floraison</t>
+  </si>
+  <si>
+    <t>NNI_F</t>
+  </si>
+  <si>
+    <t>Indice de nutrition azoté à la floraison</t>
+  </si>
+  <si>
+    <t>Nitrogen nutrition index at flowering</t>
+  </si>
+  <si>
+    <t>$max(NNI)$</t>
+  </si>
+  <si>
+    <t>NNNID_EM</t>
+  </si>
+  <si>
+    <t>Deficit azoté jusqu'à la fin floraison (discret)</t>
+  </si>
+  <si>
+    <t>Nitrogen deficit up to end of flowering (discrete)</t>
+  </si>
+  <si>
+    <t>$sum(NNI &lt; 0.8)$</t>
+  </si>
+  <si>
+    <t>NNNIE_EM</t>
+  </si>
+  <si>
+    <t>Excès azoté jusqu'à la fin floraison (discret)</t>
+  </si>
+  <si>
+    <t>Nitrogen excess up to end of flowering (discrete)</t>
+  </si>
+  <si>
+    <t>$sum(NNI &gt; 1.2)$</t>
+  </si>
+  <si>
+    <t>STDM_F</t>
+  </si>
+  <si>
+    <t>Biomasse aerienne à la floraison</t>
+  </si>
+  <si>
+    <t>Aerial Biomass at flowering</t>
+  </si>
+  <si>
+    <t>$max(TDM$</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2504,7 @@
   </sheetPr>
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -7760,579 +7992,528 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.3826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.984693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>463</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>464</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="0" t="s">
+        <v>466</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="C3" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="C4" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="I4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>474</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="0" t="s">
+      <c r="C7" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
+      <c r="A8" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>482</v>
+      <c r="C9" s="3" t="s">
+        <v>487</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>488</v>
+      <c r="F9" s="0" t="s">
+        <v>489</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="I9" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
+      <c r="A10" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C10" s="0" t="s">
         <v>491</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>492</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>492</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="F10" s="3" t="s">
         <v>493</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>494</v>
+      </c>
       <c r="G10" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="I10" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
+      <c r="A11" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C11" s="0" t="s">
         <v>491</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>496</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>496</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="F11" s="3" t="s">
         <v>497</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>498</v>
+      </c>
       <c r="G11" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="I11" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="I11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
+      <c r="A12" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C12" s="0" t="s">
         <v>491</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>500</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>500</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="F12" s="3" t="s">
         <v>497</v>
       </c>
+      <c r="F12" s="0" t="s">
+        <v>501</v>
+      </c>
       <c r="G12" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>502</v>
-      </c>
-      <c r="I12" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
+      <c r="A13" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C13" s="0" t="s">
         <v>491</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>503</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>503</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="F13" s="3" t="s">
         <v>504</v>
       </c>
+      <c r="F13" s="0" t="s">
+        <v>505</v>
+      </c>
       <c r="G13" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>506</v>
-      </c>
-      <c r="I13" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>13</v>
+      <c r="A14" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>507</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>512</v>
-      </c>
-      <c r="I14" s="0" t="s">
+      <c r="B15" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J14" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B17" s="0" t="s">
         <v>513</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="C17" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>528</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
       <c r="B18" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C18" s="0" t="s">
         <v>530</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>459</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>459</v>
@@ -8340,179 +8521,161 @@
       <c r="E18" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>459</v>
+      <c r="F18" s="0" t="s">
+        <v>531</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="I18" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="I18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>18</v>
+      <c r="A19" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C19" s="0" t="s">
         <v>530</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>533</v>
+      </c>
       <c r="D19" s="3" t="s">
-        <v>533</v>
+        <v>460</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>460</v>
+      <c r="F19" s="0" t="s">
+        <v>534</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="I19" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>19</v>
+      <c r="A20" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C20" s="0" t="s">
         <v>530</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>536</v>
+      </c>
       <c r="D20" s="3" t="s">
-        <v>536</v>
+        <v>462</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>462</v>
+      <c r="F20" s="0" t="s">
+        <v>537</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="I20" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="I20" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
+      <c r="A21" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C21" s="0" t="s">
         <v>530</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>539</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>539</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="F21" s="3" t="s">
         <v>461</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>540</v>
+      </c>
       <c r="G21" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="I21" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="I21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>21</v>
+      <c r="A22" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>546</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>547</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>22</v>
-      </c>
       <c r="B23" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C23" s="0" t="s">
         <v>549</v>
       </c>
+      <c r="C23" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>550</v>
+        <v>114</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="3" t="s">
         <v>551</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>552</v>
+      </c>
       <c r="G23" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="I23" s="0" t="s">
         <v>554</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="I23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8533,368 +8696,369 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="1:60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.2"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.25510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.8316326530612"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.89795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="43.5765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.7755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.5765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.7755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.8418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6836734693878"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>555</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>559</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
+        <v>560</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>560</v>
-      </c>
+        <v>561</v>
+      </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>567</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>562</v>
       </c>
-      <c r="D2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>563</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>562</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>572</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>571</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>572</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>570</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>576</v>
+        <v>134</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>134</v>
+        <v>578</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
+      <c r="A5" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>566</v>
+        <v>580</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>580</v>
+        <v>134</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>134</v>
+        <v>582</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>581</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
+      <c r="A6" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>570</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>91</v>
+        <v>584</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>584</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>586</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>570</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>566</v>
+        <v>590</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
+      <c r="A8" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>570</v>
-      </c>
       <c r="E8" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>592</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>593</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>595</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
+      <c r="A9" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>570</v>
-      </c>
       <c r="E9" s="0" t="s">
-        <v>564</v>
+        <v>584</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>566</v>
+        <v>599</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>91</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
+      <c r="A10" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>601</v>
-      </c>
       <c r="E10" s="0" t="s">
-        <v>91</v>
+        <v>584</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>602</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>566</v>
+        <v>603</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>91</v>
@@ -8904,388 +9068,1753 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
+      <c r="A11" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>582</v>
+        <v>606</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>601</v>
-      </c>
       <c r="E11" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>611</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>613</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>617</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="J13" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>606</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>628</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>630</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>631</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="F17" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>633</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>634</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>635</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>637</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="H19" s="0" t="s">
         <v>518</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>607</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>609</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>610</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>611</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>613</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>614</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>615</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>616</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>618</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>620</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>618</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>623</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>624</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>626</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>627</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>628</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>618</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>630</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>631</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>632</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>618</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>634</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>635</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>636</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>638</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>613</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>639</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>640</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>641</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>642</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>52</v>
+        <v>643</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>643</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>19</v>
+      <c r="A20" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>645</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>646</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>644</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>546</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>547</v>
-      </c>
       <c r="J20" s="0" t="s">
-        <v>548</v>
+        <v>647</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>645</v>
+        <v>562</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
+      <c r="A21" s="0" t="s">
+        <v>562</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>618</v>
+        <v>648</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="F21" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>650</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>649</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>653</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>649</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>657</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>658</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>665</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G27" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>646</v>
+      <c r="F28" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>673</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>707</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>708</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="K57" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>711</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>718</v>
+      </c>
+      <c r="K59" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>719</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>720</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected genotypic parameter table
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
     <sheet name="indicators" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
@@ -55,6 +55,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -2603,8 +2604,8 @@
   </sheetPr>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -8034,7 +8035,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R102"/>
+  <autoFilter ref="A1:V102"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -8918,7 +8919,7 @@
   </sheetPr>
   <dimension ref="1:85"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated rsunflo::indicate with 8 new indicators (quantitative high/low temp effect on 4 periods).
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,9 +16,9 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$R$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$V$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
@@ -58,6 +58,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="809">
   <si>
     <t>name.rsunflo.fr</t>
   </si>
@@ -2033,7 +2034,7 @@
     <t>NHT</t>
   </si>
   <si>
-    <t>Nombre de jours de hautes tempértures</t>
+    <t>Nombre de jours de hautes températures</t>
   </si>
   <si>
     <t>Thermal stress, high temperature (discrete)</t>
@@ -2045,7 +2046,7 @@
     <t>NLT</t>
   </si>
   <si>
-    <t>Nombre de jours de basses butes tempértures</t>
+    <t>Nombre de jours de basses températures</t>
   </si>
   <si>
     <t>Thermal stress, low temperature (discrete)</t>
@@ -2054,6 +2055,30 @@
     <t>$sum(TM &lt; 20)$</t>
   </si>
   <si>
+    <t>SHT</t>
+  </si>
+  <si>
+    <t>Effet des hautes températures sur la photosynthèse</t>
+  </si>
+  <si>
+    <t>Thermal stress, high temperature (continuous)</t>
+  </si>
+  <si>
+    <t>$sum(1-HTRUE)$</t>
+  </si>
+  <si>
+    <t>SLT</t>
+  </si>
+  <si>
+    <t>Effet des basses températures sur la photosynthèse</t>
+  </si>
+  <si>
+    <t>Thermal stress, low temperature (continuous)</t>
+  </si>
+  <si>
+    <t>$sum(1-LTRUE)$</t>
+  </si>
+  <si>
     <t>SFTRUE</t>
   </si>
   <si>
@@ -2351,13 +2376,37 @@
     <t>Nombre de jours chauds</t>
   </si>
   <si>
-    <t>Thermal stress, heath (discrete)</t>
+    <t>Thermal stress, heat (discrete)</t>
   </si>
   <si>
     <t>NHT_FM</t>
   </si>
   <si>
     <t>NHT_MH</t>
+  </si>
+  <si>
+    <t>SLT_EF</t>
+  </si>
+  <si>
+    <t>Thermal stress, cold (continuous)</t>
+  </si>
+  <si>
+    <t>SLT_FM</t>
+  </si>
+  <si>
+    <t>SLT_MH</t>
+  </si>
+  <si>
+    <t>SHT_EF</t>
+  </si>
+  <si>
+    <t>Thermal stress, heat (continuous)</t>
+  </si>
+  <si>
+    <t>SHT_FM</t>
+  </si>
+  <si>
+    <t>SHT_MH</t>
   </si>
   <si>
     <t>SNAB_EF</t>
@@ -2603,11 +2652,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,29 +2780,29 @@
   </sheetPr>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.1377551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.0561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="115.551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="70.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.8163265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.1581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="14.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="28.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.0204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.8367346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="130.489795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="79.5561224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.1785714285714"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="16.9183673469388"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8209,18 +8258,18 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.8418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="16.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8744,16 +8793,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.219387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="70.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="14.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.7755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="79.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="16.7397959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9440,23 +9489,23 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:85"/>
+  <dimension ref="1:93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.1581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.4387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.9795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.6173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="62.6377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="58.1377551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.7602040816326"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="16.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9846,7 +9895,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>606</v>
       </c>
@@ -9881,7 +9930,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>606</v>
       </c>
@@ -9916,7 +9965,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>606</v>
       </c>
@@ -9927,10 +9976,10 @@
         <v>627</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>615</v>
+        <v>628</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>94</v>
+        <v>610</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>665</v>
@@ -9962,25 +10011,25 @@
         <v>627</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>615</v>
+        <v>628</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>94</v>
+        <v>610</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>669</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="K15" s="0" t="s">
         <v>606</v>
@@ -10003,19 +10052,19 @@
         <v>94</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="K16" s="0" t="s">
         <v>606</v>
@@ -10029,28 +10078,28 @@
         <v>652</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>615</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>675</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>677</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>678</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>606</v>
@@ -10064,28 +10113,28 @@
         <v>652</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>615</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F18" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>680</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="I18" s="0" t="s">
+        <v>637</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>682</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>683</v>
       </c>
       <c r="K18" s="0" t="s">
         <v>606</v>
@@ -10096,28 +10145,28 @@
         <v>606</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>684</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="G19" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>685</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>686</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>687</v>
@@ -10134,10 +10183,10 @@
         <v>652</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>684</v>
+        <v>615</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>610</v>
@@ -10166,28 +10215,28 @@
         <v>606</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>693</v>
+        <v>560</v>
       </c>
       <c r="H21" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>694</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="J21" s="0" t="s">
         <v>695</v>
@@ -10201,31 +10250,31 @@
         <v>606</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>458</v>
+        <v>652</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>94</v>
+        <v>692</v>
       </c>
       <c r="E22" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>696</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>573</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>697</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>575</v>
+        <v>698</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>606</v>
@@ -10236,31 +10285,31 @@
         <v>606</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>458</v>
+        <v>652</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>94</v>
+        <v>692</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>696</v>
+        <v>610</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>606</v>
@@ -10271,28 +10320,28 @@
         <v>606</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>607</v>
+        <v>458</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>639</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>609</v>
+        <v>94</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>696</v>
+        <v>704</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>703</v>
+        <v>573</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>705</v>
+        <v>575</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>521</v>
+        <v>94</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>706</v>
@@ -10315,7 +10364,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>610</v>
+        <v>704</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>707</v>
@@ -10327,7 +10376,7 @@
         <v>709</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>392</v>
+        <v>94</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>710</v>
@@ -10341,16 +10390,16 @@
         <v>606</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>458</v>
+        <v>607</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>639</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>94</v>
+        <v>609</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>610</v>
+        <v>704</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>711</v>
@@ -10362,7 +10411,7 @@
         <v>713</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>423</v>
+        <v>521</v>
       </c>
       <c r="J26" s="0" t="s">
         <v>714</v>
@@ -10385,22 +10434,22 @@
         <v>94</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>715</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>589</v>
-      </c>
       <c r="G27" s="0" t="s">
-        <v>591</v>
+        <v>716</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>592</v>
+        <v>717</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>593</v>
+        <v>392</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>606</v>
@@ -10420,22 +10469,22 @@
         <v>94</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>715</v>
+        <v>610</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>117</v>
+        <v>719</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>597</v>
+        <v>720</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>598</v>
+        <v>721</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>599</v>
+        <v>423</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="K28" s="0" t="s">
         <v>606</v>
@@ -10443,77 +10492,77 @@
     </row>
     <row r="29" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>718</v>
+        <v>606</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>607</v>
+        <v>458</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>608</v>
+        <v>639</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>609</v>
+        <v>94</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>610</v>
+        <v>723</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>719</v>
+        <v>589</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>612</v>
+        <v>591</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>613</v>
+        <v>592</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>521</v>
+        <v>593</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>614</v>
+        <v>724</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>643</v>
+        <v>606</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>718</v>
+        <v>606</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>607</v>
+        <v>458</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>608</v>
+        <v>639</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>609</v>
+        <v>94</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>610</v>
+        <v>723</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>720</v>
+        <v>117</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>613</v>
+        <v>598</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>521</v>
+        <v>599</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>614</v>
+        <v>725</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>647</v>
+        <v>606</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>607</v>
@@ -10528,7 +10577,7 @@
         <v>610</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>721</v>
+        <v>727</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>612</v>
@@ -10543,12 +10592,12 @@
         <v>614</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>607</v>
@@ -10557,33 +10606,33 @@
         <v>608</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>94</v>
+        <v>610</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>26</v>
+        <v>612</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>137</v>
+        <v>521</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>607</v>
@@ -10592,33 +10641,33 @@
         <v>608</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>94</v>
+        <v>610</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>723</v>
+        <v>729</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>26</v>
+        <v>612</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>137</v>
+        <v>521</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>607</v>
@@ -10633,7 +10682,7 @@
         <v>94</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>26</v>
@@ -10648,12 +10697,12 @@
         <v>618</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>607</v>
@@ -10668,27 +10717,27 @@
         <v>94</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>725</v>
+        <v>731</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>620</v>
+        <v>26</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>137</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>607</v>
@@ -10703,27 +10752,27 @@
         <v>94</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>620</v>
+        <v>26</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>137</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>607</v>
@@ -10738,7 +10787,7 @@
         <v>94</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>620</v>
@@ -10753,12 +10802,12 @@
         <v>622</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>607</v>
@@ -10773,27 +10822,27 @@
         <v>94</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>728</v>
+        <v>734</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>137</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>607</v>
@@ -10808,27 +10857,27 @@
         <v>94</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>729</v>
+        <v>735</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>137</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>607</v>
@@ -10843,7 +10892,7 @@
         <v>94</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>730</v>
+        <v>736</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>624</v>
@@ -10858,18 +10907,18 @@
         <v>626</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>615</v>
@@ -10878,33 +10927,33 @@
         <v>94</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>731</v>
+        <v>737</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>666</v>
+        <v>624</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>667</v>
+        <v>625</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>670</v>
+        <v>626</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>615</v>
@@ -10913,27 +10962,27 @@
         <v>94</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>732</v>
+        <v>738</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>666</v>
+        <v>624</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>667</v>
+        <v>625</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>670</v>
+        <v>626</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>652</v>
@@ -10948,27 +10997,27 @@
         <v>94</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>666</v>
+        <v>674</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>667</v>
+        <v>675</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>652</v>
@@ -10983,27 +11032,27 @@
         <v>94</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>652</v>
@@ -11018,27 +11067,27 @@
         <v>94</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>652</v>
@@ -11053,27 +11102,27 @@
         <v>94</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>672</v>
+        <v>680</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>637</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>652</v>
@@ -11088,27 +11137,27 @@
         <v>94</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>666</v>
+        <v>680</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>667</v>
+        <v>681</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>94</v>
+        <v>637</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>668</v>
+        <v>682</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>652</v>
@@ -11123,27 +11172,27 @@
         <v>94</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>666</v>
+        <v>680</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>667</v>
+        <v>681</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>94</v>
+        <v>637</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>668</v>
+        <v>682</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>652</v>
@@ -11158,97 +11207,97 @@
         <v>94</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>666</v>
+        <v>674</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>667</v>
+        <v>675</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>668</v>
+        <v>676</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>652</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>615</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>652</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>615</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>652</v>
@@ -11263,27 +11312,27 @@
         <v>610</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>681</v>
+        <v>689</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>682</v>
+        <v>690</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>683</v>
+        <v>691</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>652</v>
@@ -11295,30 +11344,30 @@
         <v>615</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>675</v>
+        <v>610</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>677</v>
+        <v>689</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>679</v>
+        <v>691</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>652</v>
@@ -11330,30 +11379,30 @@
         <v>615</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>675</v>
+        <v>610</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>677</v>
+        <v>689</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>679</v>
+        <v>691</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>652</v>
@@ -11365,106 +11414,106 @@
         <v>615</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>679</v>
+        <v>687</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>629</v>
+        <v>683</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>631</v>
+        <v>685</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>632</v>
+        <v>686</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>633</v>
+        <v>687</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>639</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>629</v>
+        <v>683</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>631</v>
+        <v>685</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>632</v>
+        <v>686</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>633</v>
+        <v>687</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>643</v>
+        <v>651</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>607</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>628</v>
@@ -11473,7 +11522,7 @@
         <v>629</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>631</v>
@@ -11481,19 +11530,19 @@
       <c r="H58" s="0" t="s">
         <v>632</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I58" s="0" t="s">
         <v>53</v>
       </c>
       <c r="J58" s="0" t="s">
         <v>633</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>607</v>
@@ -11508,7 +11557,7 @@
         <v>629</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>631</v>
@@ -11523,82 +11572,82 @@
         <v>633</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>628</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>610</v>
+        <v>629</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>662</v>
+        <v>631</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>663</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>94</v>
+        <v>632</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>664</v>
+        <v>633</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>628</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>610</v>
+        <v>629</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>662</v>
+        <v>631</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>663</v>
+        <v>632</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>664</v>
+        <v>633</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>652</v>
@@ -11613,27 +11662,27 @@
         <v>610</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>662</v>
+        <v>670</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>663</v>
+        <v>671</v>
       </c>
       <c r="I62" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>664</v>
+        <v>672</v>
       </c>
       <c r="K62" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>652</v>
@@ -11648,27 +11697,27 @@
         <v>610</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>754</v>
+        <v>670</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>755</v>
+        <v>671</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>652</v>
@@ -11683,27 +11732,27 @@
         <v>610</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>754</v>
+        <v>670</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>755</v>
+        <v>671</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>652</v>
@@ -11718,13 +11767,13 @@
         <v>610</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>754</v>
+        <v>762</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>755</v>
+        <v>763</v>
       </c>
       <c r="I65" s="0" t="s">
         <v>637</v>
@@ -11733,12 +11782,12 @@
         <v>660</v>
       </c>
       <c r="K65" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>652</v>
@@ -11753,27 +11802,27 @@
         <v>610</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="I66" s="0" t="s">
         <v>637</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>652</v>
@@ -11788,27 +11837,27 @@
         <v>610</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="I67" s="0" t="s">
         <v>637</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>652</v>
@@ -11823,13 +11872,13 @@
         <v>610</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>759</v>
+        <v>767</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>760</v>
+        <v>768</v>
       </c>
       <c r="I68" s="0" t="s">
         <v>637</v>
@@ -11838,152 +11887,152 @@
         <v>656</v>
       </c>
       <c r="K68" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>94</v>
+        <v>610</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>560</v>
+        <v>767</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>561</v>
+        <v>768</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>686</v>
+        <v>637</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>764</v>
+        <v>656</v>
       </c>
       <c r="K69" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>94</v>
+        <v>610</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>560</v>
+        <v>767</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>561</v>
+        <v>768</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>686</v>
+        <v>637</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>764</v>
+        <v>656</v>
       </c>
       <c r="K70" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E71" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>772</v>
+      </c>
+      <c r="I71" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F71" s="0" t="s">
-        <v>766</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>686</v>
-      </c>
       <c r="J71" s="0" t="s">
-        <v>764</v>
+        <v>668</v>
       </c>
       <c r="K71" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E72" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>772</v>
+      </c>
+      <c r="I72" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F72" s="0" t="s">
-        <v>767</v>
-      </c>
-      <c r="G72" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="H72" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>686</v>
-      </c>
       <c r="J72" s="0" t="s">
-        <v>764</v>
+        <v>668</v>
       </c>
       <c r="K72" s="0" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>652</v>
@@ -11992,33 +12041,33 @@
         <v>627</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>610</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>769</v>
+        <v>666</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="I73" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>771</v>
+        <v>668</v>
       </c>
       <c r="K73" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>652</v>
@@ -12027,33 +12076,33 @@
         <v>627</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>610</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>773</v>
+        <v>662</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>775</v>
+        <v>664</v>
       </c>
       <c r="K74" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>652</v>
@@ -12062,33 +12111,33 @@
         <v>627</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>610</v>
       </c>
       <c r="F75" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="H75" s="0" t="s">
         <v>776</v>
       </c>
-      <c r="G75" s="0" t="s">
-        <v>777</v>
-      </c>
-      <c r="H75" s="0" t="s">
-        <v>778</v>
-      </c>
       <c r="I75" s="0" t="s">
-        <v>637</v>
+        <v>94</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>779</v>
+        <v>664</v>
       </c>
       <c r="K75" s="0" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>652</v>
@@ -12097,173 +12146,173 @@
         <v>627</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>684</v>
+        <v>628</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>610</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>689</v>
+        <v>662</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>690</v>
+        <v>776</v>
       </c>
       <c r="I76" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>691</v>
+        <v>664</v>
       </c>
       <c r="K76" s="0" t="s">
-        <v>643</v>
+        <v>651</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>689</v>
+        <v>560</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>690</v>
+        <v>561</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>94</v>
+        <v>694</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>691</v>
+        <v>780</v>
       </c>
       <c r="K77" s="0" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>689</v>
+        <v>560</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>690</v>
+        <v>561</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>94</v>
+        <v>694</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>691</v>
+        <v>780</v>
       </c>
       <c r="K78" s="0" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>693</v>
+        <v>560</v>
       </c>
       <c r="H79" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="I79" s="0" t="s">
         <v>694</v>
       </c>
-      <c r="I79" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="J79" s="0" t="s">
-        <v>695</v>
+        <v>780</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>652</v>
+        <v>607</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>627</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>610</v>
+        <v>94</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>693</v>
+        <v>560</v>
       </c>
       <c r="H80" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="I80" s="0" t="s">
         <v>694</v>
       </c>
-      <c r="I80" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="J80" s="0" t="s">
-        <v>695</v>
+        <v>780</v>
       </c>
       <c r="K80" s="0" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>652</v>
@@ -12272,95 +12321,95 @@
         <v>627</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>610</v>
       </c>
       <c r="F81" s="0" t="s">
+        <v>784</v>
+      </c>
+      <c r="G81" s="0" t="s">
         <v>785</v>
       </c>
-      <c r="G81" s="0" t="s">
-        <v>693</v>
-      </c>
       <c r="H81" s="0" t="s">
-        <v>694</v>
+        <v>786</v>
       </c>
       <c r="I81" s="0" t="s">
         <v>94</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>695</v>
+        <v>787</v>
       </c>
       <c r="K81" s="0" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>609</v>
+        <v>692</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>696</v>
+        <v>610</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>704</v>
+        <v>789</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>705</v>
+        <v>790</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>521</v>
+        <v>637</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>706</v>
+        <v>791</v>
       </c>
       <c r="K82" s="0" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>609</v>
+        <v>692</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>696</v>
+        <v>610</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>704</v>
+        <v>793</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>705</v>
+        <v>794</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>521</v>
+        <v>637</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>706</v>
+        <v>795</v>
       </c>
       <c r="K83" s="0" t="s">
         <v>647</v>
@@ -12368,71 +12417,351 @@
     </row>
     <row r="84" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>609</v>
+        <v>692</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>696</v>
+        <v>610</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>788</v>
+        <v>796</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="I84" s="0" t="s">
-        <v>521</v>
+        <v>94</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="K84" s="0" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>458</v>
+        <v>652</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>94</v>
+        <v>692</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>610</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>789</v>
+        <v>797</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>790</v>
+        <v>697</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>791</v>
+        <v>698</v>
       </c>
       <c r="I85" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J85" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="K85" s="0" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>798</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J86" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="K86" s="0" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>799</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J87" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="K87" s="0" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J88" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="K88" s="0" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>801</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J89" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="K89" s="0" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="J90" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="K90" s="0" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="J91" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="K91" s="0" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="J92" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="K92" s="0" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>805</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="H93" s="0" t="s">
+        <v>807</v>
+      </c>
+      <c r="I93" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="J85" s="0" t="s">
-        <v>792</v>
-      </c>
-      <c r="K85" s="0" t="s">
+      <c r="J93" s="0" t="s">
+        <v>808</v>
+      </c>
+      <c r="K93" s="0" t="s">
         <v>647</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated soil bulk density definition
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -21,9 +21,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
@@ -63,6 +63,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -568,10 +569,10 @@
     <t>SoilDensity</t>
   </si>
   <si>
-    <t>Densité apparente du sol dans l'horizon de surface (0 - 30 cm)</t>
-  </si>
-  <si>
-    <t>Soil bulk density (0-30cm)</t>
+    <t>Densité apparente du sol (tamisé, &lt; 5mm) dans l'horizon de surface (0 - 30 cm)</t>
+  </si>
+  <si>
+    <t>Soil bulk density, sieved &lt; 5mm, 0-30cm layer</t>
   </si>
   <si>
     <t>$g.cm^{-3}$</t>
@@ -586,10 +587,10 @@
     <t>soil_density_2</t>
   </si>
   <si>
-    <t>Densité apparente du sol dans l'horizon inférieur (30 cm - profondeur)</t>
-  </si>
-  <si>
-    <t>Soil bulk density (30 cm-rooting depth)</t>
+    <t>Densité apparente du sol (tamisé, &lt; 5mm) dans l'horizon inférieur (30 cm - profondeur)</t>
+  </si>
+  <si>
+    <t>Soil bulk density, sieved &lt; 5mm, 30 cm-rooting depth layer</t>
   </si>
   <si>
     <t>TC</t>
@@ -2672,16 +2673,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="K21:L22 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="85.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.4540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="96.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="29.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2806,28 +2807,27 @@
   <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="57.0561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="46.6173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.4387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="40.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="54.8979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="212.744897959184"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="129.591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="48.7755102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="43.9183673469388"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3367346938775"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="25.1989795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="31.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="64.4336734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="52.734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.2959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="45.719387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="61.9183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="240.285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="146.510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="55.0765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="33.1173469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="28.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="41.3979591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="35.0969387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8305,17 +8305,17 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="1" sqref="K21:L22 A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.0969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="89.4540816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.9948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="101.15306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.7755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="29.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8834,21 +8834,21 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K21:L22 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="129.591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="70.9132653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.3367346938775"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.4336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.7551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.7755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="146.510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.9132653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.2142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9538,20 +9538,20 @@
   <dimension ref="1:93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+      <selection pane="topLeft" activeCell="A77" activeCellId="1" sqref="K21:L22 A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.0969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="101.69387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="94.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.3979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="53.2755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="35.8163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="41.3979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="114.831632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="106.734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="46.6173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="60.2959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="29.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modified soil parameter documentation
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,9 +24,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
@@ -66,6 +66,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -511,7 +512,7 @@
     <t>Humidité massique à la capacité au champ dans l'horizon de surface (0 - 30 cm)</t>
   </si>
   <si>
-    <t>Water content at field capacity (0-30 cm)</t>
+    <t>Gravimetric water content at field capacity (0-30 cm)</t>
   </si>
   <si>
     <t>$\%$</t>
@@ -529,7 +530,7 @@
     <t>Humidité massique au point de flétrissement dans l'horizon de surface (0 - 30 cm)</t>
   </si>
   <si>
-    <t>Water content at wilting point (0-30cm)</t>
+    <t>Gravimetric water content at wilting point (0-30cm)</t>
   </si>
   <si>
     <t>Hcc_C2</t>
@@ -544,7 +545,7 @@
     <t>Humidité massique à la capacité au champ dans l'horizon inférieur (30 cm - profondeur)</t>
   </si>
   <si>
-    <t>Water content at field capacity (30 cm-rooting depth)</t>
+    <t>Gravimetric water content at field capacity (30 cm-rooting depth)</t>
   </si>
   <si>
     <t>Hpf_C2</t>
@@ -559,7 +560,7 @@
     <t>Humidité massique au point de flétrissement dans l'horizon inférieur (30 cm - profondeur)</t>
   </si>
   <si>
-    <t>Water content at wilting point (30 cm-rooting depth)</t>
+    <t>Gravimetric  water content at wilting point (30 cm-rooting depth)</t>
   </si>
   <si>
     <t>da_C1</t>
@@ -2684,16 +2685,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="L17:L20 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="123.474489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="37.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="139.489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="42.4795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,34 +2818,34 @@
   </sheetPr>
   <dimension ref="A1:W102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J69" activeCellId="0" sqref="J69"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.219387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.3163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="103.494897959184"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="72.7142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3979591836735"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.719387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="10.9795918367347"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="116.994897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="82.0765306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.8163265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3971,7 +3972,7 @@
       <c r="K17" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="L17" s="0" t="s">
+      <c r="L17" s="4" t="s">
         <v>144</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -4031,7 +4032,7 @@
       <c r="K18" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="L18" s="0" t="s">
+      <c r="L18" s="4" t="s">
         <v>150</v>
       </c>
       <c r="M18" s="4" t="s">
@@ -4091,7 +4092,7 @@
       <c r="K19" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="L19" s="0" t="s">
+      <c r="L19" s="4" t="s">
         <v>155</v>
       </c>
       <c r="M19" s="4" t="s">
@@ -4151,7 +4152,7 @@
       <c r="K20" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="L20" s="0" t="s">
+      <c r="L20" s="4" t="s">
         <v>160</v>
       </c>
       <c r="M20" s="4" t="s">
@@ -8627,19 +8628,19 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="1" sqref="L17:L20 E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.73979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="37.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="42.4795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9302,21 +9303,21 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L17:L20 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.89795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.9540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="93.7755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.0969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="187.188775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="101.872448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4132653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="95.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.015306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.2959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="211.484693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="115.015306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.1326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="47.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.9795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10006,20 +10007,20 @@
   <dimension ref="1:93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+      <selection pane="topLeft" activeCell="A77" activeCellId="1" sqref="L17:L20 A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="37.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="45.719387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="52.734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="146.688775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="136.433673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="59.3979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="77.0357142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="37.6173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="42.4795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="51.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="59.3979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="165.770408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="154.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="66.9540816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="86.9336734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="42.4795918367347"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added new metrics for model evaluation from [@Wallach2014]. updated evaluation plots : classical observed=f(simulated) and residuals plots.
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,9 +27,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$V$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
@@ -69,6 +69,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$R$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -2698,18 +2699,18 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.45408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.6173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="12.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2839,28 +2840,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.219387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.9795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.219387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="149.392857142857"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="104.755102040816"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="45.719387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="31.5"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="9.89795918367347"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="25.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.7602040816326"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.7397959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="168.831632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="118.433673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="51.4744897959184"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.4591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0408163265306"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="20.6989795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.8775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="10.9795918367347"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.9795918367347"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8649,12 +8650,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="101.69387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.719387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="114.831632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.89795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9316,20 +9318,22 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="122.571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="135.173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="89.4540816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="270.163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="146.872448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="108.892857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="60.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.4948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.89795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10024,17 +10028,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.219387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.719387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.6989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.4795918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.89795918367347"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update documentation for VLE 2.0, added reproductible example.
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,9 +37,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$W$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$W$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$W$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$W$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$W$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$W$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
@@ -79,6 +79,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">parameters!$A$1:$S$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1979,7 +1980,7 @@
     <t xml:space="preserve">Facteur de contrainte hydrique</t>
   </si>
   <si>
-    <t xml:space="preserve">Water stress index</t>
+    <t xml:space="preserve">Fraction of transpirable soil water</t>
   </si>
   <si>
     <t xml:space="preserve">FHTR</t>
@@ -3041,7 +3042,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.5"/>
@@ -3172,11 +3173,11 @@
   </sheetPr>
   <dimension ref="A1:X102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N93" activeCellId="0" sqref="N93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
@@ -9407,7 +9408,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.88"/>
@@ -10077,11 +10078,11 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.13"/>
@@ -10785,7 +10786,7 @@
       <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.26"/>
@@ -14078,7 +14079,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>

</xml_diff>

<commit_message>
removed rvle as package dependency
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="climate" sheetId="1" state="visible" r:id="rId2"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2634" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2634" uniqueCount="916">
   <si>
     <t xml:space="preserve">name.rsunflo.fr</t>
   </si>
@@ -2198,7 +2198,7 @@
     <t xml:space="preserve">$sum(RR)$</t>
   </si>
   <si>
-    <t xml:space="preserve">SETP</t>
+    <t xml:space="preserve">SPET</t>
   </si>
   <si>
     <t xml:space="preserve">Evapotranspiration</t>
@@ -2372,13 +2372,13 @@
     <t xml:space="preserve">$sum(1-FTSW)$</t>
   </si>
   <si>
-    <t xml:space="preserve">METR</t>
+    <t xml:space="preserve">MET</t>
   </si>
   <si>
     <t xml:space="preserve">$mean(ET/PET)$</t>
   </si>
   <si>
-    <t xml:space="preserve">NETR</t>
+    <t xml:space="preserve">NET</t>
   </si>
   <si>
     <t xml:space="preserve">Déficit hydrique édaphique (discret)</t>
@@ -2537,13 +2537,13 @@
     <t xml:space="preserve">SRR_MH</t>
   </si>
   <si>
-    <t xml:space="preserve">SETP_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SETP_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SETP_MH</t>
+    <t xml:space="preserve">SPET_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPET_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPET_MH</t>
   </si>
   <si>
     <t xml:space="preserve">SCWD_EF</t>
@@ -2555,13 +2555,214 @@
     <t xml:space="preserve">SCWD_MH</t>
   </si>
   <si>
-    <t xml:space="preserve">METR_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METR_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METR_MH</t>
+    <t xml:space="preserve">MET_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MET_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MET_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NET_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NET_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NET_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFTSW_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFTSW_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFTSW_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFHRUE_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFHRUE_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFHRUE_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFHTR_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFHTR_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFHTR_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFTRUE_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFTRUE_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFTRUE_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLT_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de jours froids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal stress, cold (discrete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLT_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLT_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHT_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de jours chauds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal stress, heat (discrete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHT_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHT_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLT_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal stress, cold (continuous)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLT_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLT_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHT_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal stress, heat (continuous)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHT_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHT_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNAB_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$max(NAB)$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNAB_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNAB_EM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNAB_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NNI_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice de nutrition azoté à la floraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen nutrition index at flowering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$max(NNI)$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NNNID_EM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deficit azoté jusqu'à la fin floraison (discret)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen deficit up to end of flowering (discrete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$sum(NNI &lt; 0.8)$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NNNIE_EM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excès azoté jusqu'à la fin floraison (discret)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen excess up to end of flowering (discrete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$sum(NNI &gt; 1.2)$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNNI_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNNI_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNNI_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFNRUE_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFNRUE_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFNRUE_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIR_EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIR_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIR_MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STDM_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomasse aerienne à la floraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Biomass at flowering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$max(TDM$</t>
   </si>
   <si>
     <t xml:space="preserve">NETR_EF</t>
@@ -2571,198 +2772,6 @@
   </si>
   <si>
     <t xml:space="preserve">NETR_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTSW_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTSW_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTSW_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFHRUE_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFHRUE_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFHRUE_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFHTR_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFHTR_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFHTR_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTRUE_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTRUE_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTRUE_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLT_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre de jours froids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal stress, cold (discrete)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLT_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLT_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHT_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre de jours chauds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal stress, heat (discrete)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHT_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHT_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLT_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal stress, cold (continuous)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLT_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLT_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHT_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal stress, heat (continuous)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHT_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHT_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNAB_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$max(NAB)$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNAB_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNAB_EM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNAB_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NNI_F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indice de nutrition azoté à la floraison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen nutrition index at flowering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$max(NNI)$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NNNID_EM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deficit azoté jusqu'à la fin floraison (discret)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen deficit up to end of flowering (discrete)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$sum(NNI &lt; 0.8)$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NNNIE_EM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excès azoté jusqu'à la fin floraison (discret)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen excess up to end of flowering (discrete)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$sum(NNI &gt; 1.2)$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNNI_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNNI_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNNI_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFNRUE_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFNRUE_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFNRUE_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIR_EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIR_FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIR_MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STDM_F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomasse aerienne à la floraison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aerial Biomass at flowering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$max(TDM$</t>
   </si>
   <si>
     <t xml:space="preserve">STR_FH</t>
@@ -3014,7 +3023,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F17:F18 F43:F48 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3148,8 +3157,8 @@
   </sheetPr>
   <dimension ref="A1:X102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N48" activeCellId="0" sqref="N48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N48" activeCellId="2" sqref="F17:F18 F43:F48 N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9380,7 +9389,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F17:F18 F43:F48 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10054,7 +10063,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="2" sqref="F17:F18 F43:F48 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10757,8 +10766,8 @@
   </sheetPr>
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17:F18 F43:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14051,7 +14060,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F17:F18 F43:F48 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14104,7 +14113,7 @@
         <v>700</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>831</v>
+        <v>898</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>770</v>
@@ -14133,7 +14142,7 @@
         <v>700</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>832</v>
+        <v>899</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>770</v>
@@ -14162,7 +14171,7 @@
         <v>700</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>833</v>
+        <v>900</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>770</v>
@@ -14220,22 +14229,22 @@
         <v>773</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>156</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>128</v>
@@ -14249,13 +14258,13 @@
         <v>719</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>721</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>57</v>
@@ -14264,7 +14273,7 @@
         <v>723</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>128</v>
@@ -14275,7 +14284,7 @@
         <v>729</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>128</v>
@@ -14304,7 +14313,7 @@
         <v>729</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>135</v>
@@ -14391,7 +14400,7 @@
         <v>782</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>872</v>
@@ -14429,7 +14438,7 @@
         <v>882</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>727</v>
@@ -14464,7 +14473,7 @@
         <v>727</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>741</v>
@@ -14481,7 +14490,7 @@
         <v>700</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>805</v>
@@ -14510,7 +14519,7 @@
         <v>793</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>797</v>
@@ -14533,13 +14542,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>106</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
updated documentation to mention constraint on root_depth value.
</commit_message>
<xml_diff>
--- a/inst/doc/files/parameterization.xlsx
+++ b/inst/doc/files/parameterization.xlsx
@@ -533,10 +533,10 @@
     <t xml:space="preserve">RootDepthLimit</t>
   </si>
   <si>
-    <t xml:space="preserve">Profondeur d'enracinement maximale dans le sol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum soil rooting depth</t>
+    <t xml:space="preserve">Profondeur d'enracinement maximale dans le sol (&gt; 300 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum soil rooting depth (&gt; 300 mm)</t>
   </si>
   <si>
     <t xml:space="preserve">$mm$</t>
@@ -557,10 +557,10 @@
     <t xml:space="preserve">$\theta_{fc}$</t>
   </si>
   <si>
-    <t xml:space="preserve">Humidité massique à la capacité au champ dans l'horizon de surface (0 - 30 cm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gravimetric water content at field capacity (0 - 30 cm)</t>
+    <t xml:space="preserve">Humidité massique à la capacité au champ dans l'horizon de surface (0 - 300 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravimetric water content at field capacity (0 - 300 mm)</t>
   </si>
   <si>
     <t xml:space="preserve">$\%$</t>
@@ -578,10 +578,10 @@
     <t xml:space="preserve">$\theta_{wp}$</t>
   </si>
   <si>
-    <t xml:space="preserve">Humidité massique au point de flétrissement dans l'horizon de surface (0 - 30 cm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gravimetric water content at wilting point (0 - 30cm)</t>
+    <t xml:space="preserve">Humidité massique au point de flétrissement dans l'horizon de surface (0 - 300 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravimetric water content at wilting point (0 - 300 mm)</t>
   </si>
   <si>
     <t xml:space="preserve">Hcc_C2</t>
@@ -593,10 +593,10 @@
     <t xml:space="preserve">field_capacity_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Humidité massique à la capacité au champ dans l'horizon inférieur (30 cm - profondeur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gravimetric water content at field capacity (30 cm - root depth)</t>
+    <t xml:space="preserve">Humidité massique à la capacité au champ dans l'horizon inférieur (300 mm - profondeur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravimetric water content at field capacity (300 mm - root depth)</t>
   </si>
   <si>
     <t xml:space="preserve">Hpf_C2</t>
@@ -608,10 +608,10 @@
     <t xml:space="preserve">wilting_point_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Humidité massique au point de flétrissement dans l'horizon inférieur (30 cm - profondeur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gravimetric  water content at wilting point (30 cm - root depth)</t>
+    <t xml:space="preserve">Humidité massique au point de flétrissement dans l'horizon inférieur (300 mm - profondeur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravimetric  water content at wilting point (300 mm - root depth)</t>
   </si>
   <si>
     <t xml:space="preserve">da_C1</t>
@@ -626,10 +626,10 @@
     <t xml:space="preserve">SoilDensity</t>
   </si>
   <si>
-    <t xml:space="preserve">Densité apparente du sol (tamisé, &lt; 5mm) dans l'horizon de surface (0 - 30 cm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil bulk density, sieved &lt; 5mm, (0 - 30cm)</t>
+    <t xml:space="preserve">Densité apparente du sol (tamisé, &lt; 5mm) dans l'horizon de surface (0 - 300 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil bulk density, sieved &lt; 5mm, (0 - 300 mm)</t>
   </si>
   <si>
     <t xml:space="preserve">$g.cm^{-3}$</t>
@@ -644,10 +644,10 @@
     <t xml:space="preserve">soil_density_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Densité apparente du sol (tamisé, &lt; 5mm) dans l'horizon inférieur (30 cm - profondeur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil bulk density, sieved &lt; 5mm, (30 cm - root depth)</t>
+    <t xml:space="preserve">Densité apparente du sol (tamisé, &lt; 5mm) dans l'horizon inférieur (300 mm - profondeur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil bulk density, sieved &lt; 5mm, (300 mm - root depth)</t>
   </si>
   <si>
     <t xml:space="preserve">TC</t>
@@ -1130,10 +1130,10 @@
     <t xml:space="preserve">SoilNitrogenInitial</t>
   </si>
   <si>
-    <t xml:space="preserve">Reliquats azotés dans l'horizon de surface (0 - 30 cm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial value for nitrogen residuals in surface layer  (0-30 cm)</t>
+    <t xml:space="preserve">Reliquats azotés dans l'horizon de surface (0 - 300 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial value for nitrogen residuals in surface layer  (0 - 300 mm)</t>
   </si>
   <si>
     <t xml:space="preserve">$kg.ha^{-1}$</t>
@@ -1148,10 +1148,10 @@
     <t xml:space="preserve">nitrogen_initial_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Reliquats azotés dans l'horizon inférieur (30 cm - profondeur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial value for nitrogen residuals in root layer (30 cm-rooting depth)</t>
+    <t xml:space="preserve">Reliquats azotés dans l'horizon inférieur (300 mm - profondeur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial value for nitrogen residuals in root layer (300 mm - rooting depth)</t>
   </si>
   <si>
     <t xml:space="preserve">Hini_C1</t>
@@ -1169,10 +1169,10 @@
     <t xml:space="preserve">$\theta_0$</t>
   </si>
   <si>
-    <t xml:space="preserve">Valeur initiale de remplissage de la reserve hydrique (0 - 30 cm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial value for soil water capacity in surface layer  (0-30 cm)</t>
+    <t xml:space="preserve">Valeur initiale de remplissage de la reserve hydrique (0 - 300 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial value for soil water capacity in surface layer  (0 - 300 mm)</t>
   </si>
   <si>
     <t xml:space="preserve">Hini_C2</t>
@@ -1184,10 +1184,10 @@
     <t xml:space="preserve">water_initial_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Valeur initiale de remplissage de la reserve hydrique (30 cm – profondeur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial value for soil water capacity in root layer (30 cm-rooting depth)</t>
+    <t xml:space="preserve">Valeur initiale de remplissage de la reserve hydrique (300 mm - profondeur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial value for soil water capacity in root layer (300 mm - rooting depth)</t>
   </si>
   <si>
     <t xml:space="preserve">zC1</t>
@@ -2988,12 +2988,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3074,14 +3074,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.72265625" defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="20.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3206,21 +3205,21 @@
   <dimension ref="A1:Y97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A97" activeCellId="0" sqref="A97"/>
+      <selection pane="bottomRight" activeCell="N54" activeCellId="0" sqref="N54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.05"/>
@@ -3232,15 +3231,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="16.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="16.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="16.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9659,9 +9657,8 @@
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.52"/>
@@ -9671,7 +9668,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="59.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10433,15 +10429,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.9140625" defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="79.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="43.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11107,7 +11101,7 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.9140625" defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.26"/>
@@ -11120,7 +11114,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14400,7 +14393,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
@@ -14410,7 +14403,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>